<commit_message>
added capability to translate x1-coord into eta-coord for NURBS curves
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>test #</t>
   </si>
@@ -328,13 +328,25 @@
   <si>
     <t>based off of template6</t>
   </si>
+  <si>
+    <t>shear web height at station</t>
+  </si>
+  <si>
+    <t>22-monospar</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>from monoplane_spar_layup.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -374,7 +386,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,8 +411,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -617,10 +641,21 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -629,18 +664,42 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="hair">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -661,33 +720,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -704,8 +742,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -721,16 +759,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,60 +1149,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:AK44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="31"/>
+    <col min="2" max="2" width="9.140625" style="24"/>
     <col min="3" max="3" width="26.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="14"/>
-    <col min="13" max="13" width="91.28515625" customWidth="1"/>
+    <col min="8" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="9" customWidth="1"/>
+    <col min="13" max="35" width="5.7109375" customWidth="1"/>
+    <col min="36" max="36" width="5.7109375" style="9" customWidth="1"/>
+    <col min="37" max="37" width="91.28515625" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="34" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="56"/>
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="34" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="32"/>
+    <row r="2" spans="1:37" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="32"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="33"/>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1094,28 +1240,100 @@
       <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="34"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="31">
+      <c r="M2" s="6">
+        <v>1</v>
+      </c>
+      <c r="N2" s="39">
+        <v>2</v>
+      </c>
+      <c r="O2" s="38">
+        <v>3</v>
+      </c>
+      <c r="P2" s="38">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="51">
+        <v>5</v>
+      </c>
+      <c r="R2" s="38">
+        <v>6</v>
+      </c>
+      <c r="S2" s="38">
+        <v>7</v>
+      </c>
+      <c r="T2" s="38">
+        <v>8</v>
+      </c>
+      <c r="U2" s="38">
+        <v>9</v>
+      </c>
+      <c r="V2" s="38">
+        <v>10</v>
+      </c>
+      <c r="W2" s="38">
+        <v>11</v>
+      </c>
+      <c r="X2" s="38">
+        <v>12</v>
+      </c>
+      <c r="Y2" s="38">
+        <v>13</v>
+      </c>
+      <c r="Z2" s="38">
+        <v>14</v>
+      </c>
+      <c r="AA2" s="38">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="38">
+        <v>16</v>
+      </c>
+      <c r="AC2" s="39">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>19</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>20</v>
+      </c>
+      <c r="AG2" s="6">
+        <v>21</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>22</v>
+      </c>
+      <c r="AI2" s="6">
+        <v>23</v>
+      </c>
+      <c r="AJ2" s="37">
+        <v>24</v>
+      </c>
+      <c r="AK2" s="34"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1135,24 +1353,120 @@
       <c r="G3" s="4">
         <v>11</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="10">
         <v>0.215</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="10">
         <v>0.217</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="10">
         <v>0.318</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="10">
         <v>0.01</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="31">
+      <c r="M3" s="42">
+        <f>$M$24</f>
+        <v>5.266</v>
+      </c>
+      <c r="N3" s="50">
+        <f>$N$24</f>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O3" s="42">
+        <f>O$24/2</f>
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="P3" s="42">
+        <f>P$24/2</f>
+        <v>2.3704999999999998</v>
+      </c>
+      <c r="Q3" s="52">
+        <f>Q$24/2</f>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="R3" s="42">
+        <f>R$24/2</f>
+        <v>2.0455000000000001</v>
+      </c>
+      <c r="S3" s="42">
+        <f t="shared" ref="S3:Z9" si="0">S$24/2</f>
+        <v>1.84</v>
+      </c>
+      <c r="T3" s="42">
+        <f t="shared" si="0"/>
+        <v>1.74</v>
+      </c>
+      <c r="U3" s="53">
+        <f>U$24/2</f>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="V3" s="47">
+        <f>V$24/2</f>
+        <v>1.5445</v>
+      </c>
+      <c r="W3" s="48">
+        <f t="shared" ref="U3:AC8" si="1">W$24</f>
+        <v>2.8820000000000001</v>
+      </c>
+      <c r="X3" s="47">
+        <f t="shared" si="1"/>
+        <v>2.6960000000000002</v>
+      </c>
+      <c r="Y3" s="47">
+        <f t="shared" si="1"/>
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="Z3" s="47">
+        <f t="shared" si="1"/>
+        <v>2.077</v>
+      </c>
+      <c r="AA3" s="47">
+        <f t="shared" si="1"/>
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="AB3" s="47">
+        <f t="shared" si="1"/>
+        <v>1.36</v>
+      </c>
+      <c r="AC3" s="47">
+        <f t="shared" si="1"/>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="AD3" s="42">
+        <f>AD$24</f>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE3" s="42">
+        <f t="shared" ref="AE3:AJ18" si="2">AE$24</f>
+        <v>0.91</v>
+      </c>
+      <c r="AF3" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG3" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH3" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI3" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ3" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1162,34 +1476,130 @@
         <v>2</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E23" si="0">D4+3</f>
+        <f t="shared" ref="E4:E23" si="3">D4+3</f>
         <v>5</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F23" si="1">G4-2</f>
+        <f t="shared" ref="F4:F23" si="4">G4-2</f>
         <v>10</v>
       </c>
       <c r="G4" s="4">
         <v>12</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="10">
         <v>0.245</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="10">
         <v>0.24</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="10">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="31">
+      <c r="M4" s="42">
+        <f t="shared" ref="M4:M23" si="5">$M$24</f>
+        <v>5.266</v>
+      </c>
+      <c r="N4" s="50">
+        <f t="shared" ref="N4:N23" si="6">$N$24</f>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O4" s="42">
+        <f t="shared" ref="O4:P9" si="7">O$24/2</f>
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="P4" s="42">
+        <f t="shared" si="7"/>
+        <v>2.3704999999999998</v>
+      </c>
+      <c r="Q4" s="52">
+        <f t="shared" ref="Q4:R9" si="8">Q$24/2</f>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="R4" s="42">
+        <f t="shared" si="8"/>
+        <v>2.0455000000000001</v>
+      </c>
+      <c r="S4" s="42">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
+      </c>
+      <c r="T4" s="42">
+        <f t="shared" si="0"/>
+        <v>1.74</v>
+      </c>
+      <c r="U4" s="42">
+        <f t="shared" si="0"/>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="V4" s="53">
+        <f>V$24/2</f>
+        <v>1.5445</v>
+      </c>
+      <c r="W4" s="47">
+        <f>W$24/2</f>
+        <v>1.4410000000000001</v>
+      </c>
+      <c r="X4" s="48">
+        <f t="shared" si="1"/>
+        <v>2.6960000000000002</v>
+      </c>
+      <c r="Y4" s="47">
+        <f t="shared" si="1"/>
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="Z4" s="47">
+        <f t="shared" si="1"/>
+        <v>2.077</v>
+      </c>
+      <c r="AA4" s="47">
+        <f t="shared" si="1"/>
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="AB4" s="47">
+        <f t="shared" si="1"/>
+        <v>1.36</v>
+      </c>
+      <c r="AC4" s="47">
+        <f t="shared" si="1"/>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="AD4" s="42">
+        <f t="shared" ref="AD4:AJ23" si="9">AD$24</f>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE4" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF4" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG4" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH4" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI4" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ4" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B5" s="24">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1199,34 +1609,130 @@
         <v>2</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G5" s="4">
         <v>13</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="10">
         <v>0.27400000000000002</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="10">
         <v>0.214</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="10">
         <v>0.25</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="31">
+      <c r="M5" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N5" s="50">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O5" s="42">
+        <f t="shared" si="7"/>
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="P5" s="42">
+        <f t="shared" si="7"/>
+        <v>2.3704999999999998</v>
+      </c>
+      <c r="Q5" s="52">
+        <f t="shared" si="8"/>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="R5" s="42">
+        <f t="shared" si="8"/>
+        <v>2.0455000000000001</v>
+      </c>
+      <c r="S5" s="42">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
+      </c>
+      <c r="T5" s="42">
+        <f t="shared" si="0"/>
+        <v>1.74</v>
+      </c>
+      <c r="U5" s="42">
+        <f t="shared" si="0"/>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="V5" s="42">
+        <f t="shared" si="0"/>
+        <v>1.5445</v>
+      </c>
+      <c r="W5" s="53">
+        <f>W$24/2</f>
+        <v>1.4410000000000001</v>
+      </c>
+      <c r="X5" s="47">
+        <f>X$24/2</f>
+        <v>1.3480000000000001</v>
+      </c>
+      <c r="Y5" s="48">
+        <f t="shared" si="1"/>
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="Z5" s="47">
+        <f t="shared" si="1"/>
+        <v>2.077</v>
+      </c>
+      <c r="AA5" s="47">
+        <f t="shared" si="1"/>
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="AB5" s="47">
+        <f t="shared" si="1"/>
+        <v>1.36</v>
+      </c>
+      <c r="AC5" s="47">
+        <f t="shared" si="1"/>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="AD5" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE5" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF5" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG5" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH5" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI5" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ5" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B6" s="24">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1236,34 +1742,130 @@
         <v>2</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G6" s="4">
         <v>14</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="10">
         <v>0.36299999999999999</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="10">
         <v>0.32600000000000001</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="10">
         <v>0.189</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="31">
+      <c r="M6" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N6" s="50">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O6" s="42">
+        <f t="shared" si="7"/>
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="P6" s="42">
+        <f t="shared" si="7"/>
+        <v>2.3704999999999998</v>
+      </c>
+      <c r="Q6" s="52">
+        <f t="shared" si="8"/>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="R6" s="42">
+        <f t="shared" si="8"/>
+        <v>2.0455000000000001</v>
+      </c>
+      <c r="S6" s="42">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
+      </c>
+      <c r="T6" s="42">
+        <f t="shared" si="0"/>
+        <v>1.74</v>
+      </c>
+      <c r="U6" s="42">
+        <f t="shared" si="0"/>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="V6" s="42">
+        <f t="shared" si="0"/>
+        <v>1.5445</v>
+      </c>
+      <c r="W6" s="42">
+        <f t="shared" si="0"/>
+        <v>1.4410000000000001</v>
+      </c>
+      <c r="X6" s="53">
+        <f>X$24/2</f>
+        <v>1.3480000000000001</v>
+      </c>
+      <c r="Y6" s="47">
+        <f>Y$24/2</f>
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="Z6" s="48">
+        <f t="shared" si="1"/>
+        <v>2.077</v>
+      </c>
+      <c r="AA6" s="47">
+        <f t="shared" si="1"/>
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="AB6" s="47">
+        <f t="shared" si="1"/>
+        <v>1.36</v>
+      </c>
+      <c r="AC6" s="47">
+        <f t="shared" si="1"/>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="AD6" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE6" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF6" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG6" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH6" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI6" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ6" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B7" s="24">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1273,34 +1875,130 @@
         <v>2</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G7" s="4">
         <v>15</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="10">
         <v>0.45200000000000001</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="10">
         <v>0.39300000000000002</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="10">
         <v>0.152</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="31">
+      <c r="M7" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N7" s="50">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O7" s="42">
+        <f t="shared" si="7"/>
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="P7" s="42">
+        <f t="shared" si="7"/>
+        <v>2.3704999999999998</v>
+      </c>
+      <c r="Q7" s="52">
+        <f t="shared" si="8"/>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="R7" s="42">
+        <f t="shared" si="8"/>
+        <v>2.0455000000000001</v>
+      </c>
+      <c r="S7" s="42">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
+      </c>
+      <c r="T7" s="42">
+        <f t="shared" si="0"/>
+        <v>1.74</v>
+      </c>
+      <c r="U7" s="42">
+        <f t="shared" si="0"/>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="V7" s="42">
+        <f t="shared" si="0"/>
+        <v>1.5445</v>
+      </c>
+      <c r="W7" s="42">
+        <f t="shared" si="0"/>
+        <v>1.4410000000000001</v>
+      </c>
+      <c r="X7" s="42">
+        <f t="shared" si="0"/>
+        <v>1.3480000000000001</v>
+      </c>
+      <c r="Y7" s="53">
+        <f>Y$24/2</f>
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="Z7" s="47">
+        <f>Z$24/2</f>
+        <v>1.0385</v>
+      </c>
+      <c r="AA7" s="48">
+        <f t="shared" si="1"/>
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="AB7" s="47">
+        <f t="shared" si="1"/>
+        <v>1.36</v>
+      </c>
+      <c r="AC7" s="47">
+        <f t="shared" si="1"/>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="AD7" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE7" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF7" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG7" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH7" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI7" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ7" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B8" s="24">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1310,77 +2008,269 @@
         <v>2</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G8" s="4">
         <v>16</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="10">
         <v>0.54</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="10">
         <v>0.32700000000000001</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="10">
         <v>0.127</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="10">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="M8" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N8" s="50">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O8" s="42">
+        <f t="shared" si="7"/>
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="P8" s="42">
+        <f t="shared" si="7"/>
+        <v>2.3704999999999998</v>
+      </c>
+      <c r="Q8" s="52">
+        <f t="shared" si="8"/>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="R8" s="42">
+        <f t="shared" si="8"/>
+        <v>2.0455000000000001</v>
+      </c>
+      <c r="S8" s="42">
+        <f t="shared" si="0"/>
+        <v>1.84</v>
+      </c>
+      <c r="T8" s="42">
+        <f t="shared" si="0"/>
+        <v>1.74</v>
+      </c>
+      <c r="U8" s="42">
+        <f t="shared" si="0"/>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="V8" s="42">
+        <f t="shared" si="0"/>
+        <v>1.5445</v>
+      </c>
+      <c r="W8" s="42">
+        <f t="shared" si="0"/>
+        <v>1.4410000000000001</v>
+      </c>
+      <c r="X8" s="42">
+        <f t="shared" si="0"/>
+        <v>1.3480000000000001</v>
+      </c>
+      <c r="Y8" s="42">
+        <f t="shared" si="0"/>
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="Z8" s="53">
+        <f>Z$24/2</f>
+        <v>1.0385</v>
+      </c>
+      <c r="AA8" s="47">
+        <f>AA$24/2</f>
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="AB8" s="48">
+        <f t="shared" si="1"/>
+        <v>1.36</v>
+      </c>
+      <c r="AC8" s="47">
+        <f t="shared" si="1"/>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="AD8" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE8" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF8" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG8" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH8" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI8" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ8" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="16">
         <v>7</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="16">
         <v>2</v>
       </c>
       <c r="E9" s="3">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="G9" s="17">
+        <v>17</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0.629</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0.109</v>
+      </c>
+      <c r="K9" s="18">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L9" s="19">
+        <v>1</v>
+      </c>
+      <c r="M9" s="43">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N9" s="50">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O9" s="44">
+        <f t="shared" si="7"/>
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="P9" s="44">
+        <f t="shared" si="7"/>
+        <v>2.3704999999999998</v>
+      </c>
+      <c r="Q9" s="54">
+        <f t="shared" si="8"/>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="R9" s="44">
+        <f t="shared" si="8"/>
+        <v>2.0455000000000001</v>
+      </c>
+      <c r="S9" s="44">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="G9" s="24">
-        <v>17</v>
-      </c>
-      <c r="H9" s="25">
-        <v>0.629</v>
-      </c>
-      <c r="I9" s="25">
-        <v>0.28199999999999997</v>
-      </c>
-      <c r="J9" s="25">
-        <v>0.109</v>
-      </c>
-      <c r="K9" s="25">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="L9" s="26">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
+        <v>1.84</v>
+      </c>
+      <c r="T9" s="44">
+        <f t="shared" si="0"/>
+        <v>1.74</v>
+      </c>
+      <c r="U9" s="44">
+        <f t="shared" si="0"/>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="V9" s="44">
+        <f t="shared" si="0"/>
+        <v>1.5445</v>
+      </c>
+      <c r="W9" s="44">
+        <f t="shared" si="0"/>
+        <v>1.4410000000000001</v>
+      </c>
+      <c r="X9" s="44">
+        <f t="shared" si="0"/>
+        <v>1.3480000000000001</v>
+      </c>
+      <c r="Y9" s="44">
+        <f t="shared" si="0"/>
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="Z9" s="44">
+        <f t="shared" si="0"/>
+        <v>1.0385</v>
+      </c>
+      <c r="AA9" s="54">
+        <f>AA$24/2</f>
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="AB9" s="44">
+        <f>AB$24/2</f>
+        <v>0.68</v>
+      </c>
+      <c r="AC9" s="49">
+        <f>AC$24</f>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="AD9" s="44">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE9" s="44">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF9" s="44">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG9" s="44">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH9" s="44">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI9" s="44">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ9" s="45">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="AK9" s="35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="31">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B10" s="24">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1389,36 +2279,87 @@
       <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="E10" s="28">
-        <f t="shared" si="0"/>
+      <c r="E10" s="21">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="F10" s="27">
-        <f t="shared" si="1"/>
+      <c r="F10" s="20">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G10" s="4">
         <v>11</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="10">
         <v>0.215</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="10">
         <v>0.217</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="10">
         <v>0.318</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="10">
         <v>0.01</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="11">
         <v>0.75</v>
       </c>
-      <c r="M10" s="35"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="31">
+      <c r="M10" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N10" s="46">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="42"/>
+      <c r="V10" s="42"/>
+      <c r="W10" s="42"/>
+      <c r="X10" s="42"/>
+      <c r="Y10" s="42"/>
+      <c r="Z10" s="42"/>
+      <c r="AA10" s="42"/>
+      <c r="AB10" s="42"/>
+      <c r="AC10" s="42"/>
+      <c r="AD10" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE10" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF10" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG10" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH10" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI10" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ10" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="AK10" s="36"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B11" s="24">
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1428,34 +2369,85 @@
         <v>2</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G11" s="4">
         <v>12</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="10">
         <v>0.245</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="10">
         <v>0.24</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="10">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="11">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="31">
+      <c r="M11" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N11" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="42"/>
+      <c r="X11" s="42"/>
+      <c r="Y11" s="42"/>
+      <c r="Z11" s="42"/>
+      <c r="AA11" s="42"/>
+      <c r="AB11" s="42"/>
+      <c r="AC11" s="42"/>
+      <c r="AD11" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE11" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF11" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG11" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH11" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI11" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ11" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B12" s="24">
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1465,34 +2457,85 @@
         <v>2</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G12" s="4">
         <v>13</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="10">
         <v>0.27400000000000002</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="10">
         <v>0.214</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="10">
         <v>0.25</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="11">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="31">
+      <c r="M12" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N12" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="42"/>
+      <c r="X12" s="42"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="42"/>
+      <c r="AB12" s="42"/>
+      <c r="AC12" s="42"/>
+      <c r="AD12" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE12" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF12" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG12" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH12" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI12" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ12" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B13" s="24">
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1502,34 +2545,85 @@
         <v>2</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G13" s="4">
         <v>14</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="10">
         <v>0.36299999999999999</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="10">
         <v>0.32600000000000001</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="10">
         <v>0.189</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="11">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="31">
+      <c r="M13" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N13" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="42"/>
+      <c r="X13" s="42"/>
+      <c r="Y13" s="42"/>
+      <c r="Z13" s="42"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42"/>
+      <c r="AC13" s="42"/>
+      <c r="AD13" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE13" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF13" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG13" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH13" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI13" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ13" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B14" s="24">
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1539,34 +2633,85 @@
         <v>2</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G14" s="4">
         <v>15</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="10">
         <v>0.45200000000000001</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="10">
         <v>0.39300000000000002</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="10">
         <v>0.152</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="11">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="31">
+      <c r="M14" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N14" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="42"/>
+      <c r="X14" s="42"/>
+      <c r="Y14" s="42"/>
+      <c r="Z14" s="42"/>
+      <c r="AA14" s="42"/>
+      <c r="AB14" s="42"/>
+      <c r="AC14" s="42"/>
+      <c r="AD14" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE14" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF14" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG14" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH14" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI14" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ14" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B15" s="24">
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1576,72 +2721,174 @@
         <v>2</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G15" s="4">
         <v>16</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="10">
         <v>0.54</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="10">
         <v>0.32700000000000001</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="10">
         <v>0.127</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="10">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="11">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="23">
+      <c r="M15" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N15" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="42"/>
+      <c r="X15" s="42"/>
+      <c r="Y15" s="42"/>
+      <c r="Z15" s="42"/>
+      <c r="AA15" s="42"/>
+      <c r="AB15" s="42"/>
+      <c r="AC15" s="42"/>
+      <c r="AD15" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE15" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF15" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG15" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH15" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI15" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ15" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="16">
         <v>14</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="16">
         <v>2</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="17">
         <v>17</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="18">
         <v>0.629</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="18">
         <v>0.28199999999999997</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="18">
         <v>0.109</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="18">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="19">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="31">
+      <c r="M16" s="43">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N16" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="44"/>
+      <c r="X16" s="44"/>
+      <c r="Y16" s="44"/>
+      <c r="Z16" s="44"/>
+      <c r="AA16" s="44"/>
+      <c r="AB16" s="44"/>
+      <c r="AC16" s="44"/>
+      <c r="AD16" s="44">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE16" s="44">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF16" s="44">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG16" s="44">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH16" s="44">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI16" s="44">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ16" s="45">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B17" s="24">
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1650,36 +2897,87 @@
       <c r="D17" s="1">
         <v>2</v>
       </c>
-      <c r="E17" s="28">
-        <f t="shared" si="0"/>
+      <c r="E17" s="21">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="F17" s="27">
-        <f t="shared" si="1"/>
+      <c r="F17" s="20">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G17" s="4">
         <v>11</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="10">
         <v>0.215</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="10">
         <v>0.217</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="10">
         <v>0.318</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="10">
         <v>0.01</v>
       </c>
-      <c r="L17" s="17">
+      <c r="L17" s="11">
         <v>0.5</v>
       </c>
-      <c r="M17" s="35"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="31">
+      <c r="M17" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N17" s="46">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="V17" s="42"/>
+      <c r="W17" s="42"/>
+      <c r="X17" s="42"/>
+      <c r="Y17" s="42"/>
+      <c r="Z17" s="42"/>
+      <c r="AA17" s="42"/>
+      <c r="AB17" s="42"/>
+      <c r="AC17" s="42"/>
+      <c r="AD17" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE17" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF17" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG17" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH17" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI17" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ17" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="AK17" s="36"/>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B18" s="24">
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1689,34 +2987,85 @@
         <v>2</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G18" s="4">
         <v>12</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="10">
         <v>0.245</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="10">
         <v>0.24</v>
       </c>
-      <c r="J18" s="16">
+      <c r="J18" s="10">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L18" s="17">
+      <c r="L18" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="31">
+      <c r="M18" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N18" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="42"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42"/>
+      <c r="AA18" s="42"/>
+      <c r="AB18" s="42"/>
+      <c r="AC18" s="42"/>
+      <c r="AD18" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE18" s="42">
+        <f t="shared" si="2"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF18" s="42">
+        <f t="shared" si="2"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG18" s="42">
+        <f t="shared" si="2"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH18" s="42">
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI18" s="42">
+        <f t="shared" si="2"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ18" s="42">
+        <f t="shared" si="2"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B19" s="24">
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1726,34 +3075,85 @@
         <v>2</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G19" s="4">
         <v>13</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="10">
         <v>0.27400000000000002</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="10">
         <v>0.214</v>
       </c>
-      <c r="J19" s="16">
+      <c r="J19" s="10">
         <v>0.25</v>
       </c>
-      <c r="K19" s="16">
+      <c r="K19" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L19" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="31">
+      <c r="M19" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N19" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="42"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="42"/>
+      <c r="AC19" s="42"/>
+      <c r="AD19" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE19" s="42">
+        <f t="shared" si="9"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF19" s="42">
+        <f t="shared" si="9"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG19" s="42">
+        <f t="shared" si="9"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH19" s="42">
+        <f t="shared" si="9"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI19" s="42">
+        <f t="shared" si="9"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ19" s="42">
+        <f t="shared" si="9"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B20" s="24">
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1763,34 +3163,85 @@
         <v>2</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G20" s="4">
         <v>14</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="10">
         <v>0.36299999999999999</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="10">
         <v>0.32600000000000001</v>
       </c>
-      <c r="J20" s="16">
+      <c r="J20" s="10">
         <v>0.189</v>
       </c>
-      <c r="K20" s="16">
+      <c r="K20" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L20" s="17">
+      <c r="L20" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="31">
+      <c r="M20" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N20" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="42"/>
+      <c r="V20" s="42"/>
+      <c r="W20" s="42"/>
+      <c r="X20" s="42"/>
+      <c r="Y20" s="42"/>
+      <c r="Z20" s="42"/>
+      <c r="AA20" s="42"/>
+      <c r="AB20" s="42"/>
+      <c r="AC20" s="42"/>
+      <c r="AD20" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE20" s="42">
+        <f t="shared" si="9"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF20" s="42">
+        <f t="shared" si="9"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG20" s="42">
+        <f t="shared" si="9"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH20" s="42">
+        <f t="shared" si="9"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI20" s="42">
+        <f t="shared" si="9"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ20" s="42">
+        <f t="shared" si="9"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B21" s="24">
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1800,34 +3251,85 @@
         <v>2</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G21" s="4">
         <v>15</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="10">
         <v>0.45200000000000001</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="10">
         <v>0.39300000000000002</v>
       </c>
-      <c r="J21" s="16">
+      <c r="J21" s="10">
         <v>0.152</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K21" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="31">
+      <c r="M21" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N21" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="42"/>
+      <c r="W21" s="42"/>
+      <c r="X21" s="42"/>
+      <c r="Y21" s="42"/>
+      <c r="Z21" s="42"/>
+      <c r="AA21" s="42"/>
+      <c r="AB21" s="42"/>
+      <c r="AC21" s="42"/>
+      <c r="AD21" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE21" s="42">
+        <f t="shared" si="9"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF21" s="42">
+        <f t="shared" si="9"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG21" s="42">
+        <f t="shared" si="9"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH21" s="42">
+        <f t="shared" si="9"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI21" s="42">
+        <f t="shared" si="9"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ21" s="42">
+        <f t="shared" si="9"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B22" s="24">
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1837,229 +3339,431 @@
         <v>2</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G22" s="4">
         <v>16</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="10">
         <v>0.54</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="10">
         <v>0.32700000000000001</v>
       </c>
-      <c r="J22" s="16">
+      <c r="J22" s="10">
         <v>0.127</v>
       </c>
-      <c r="K22" s="16">
+      <c r="K22" s="10">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="L22" s="17">
+      <c r="L22" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="23">
+      <c r="M22" s="42">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N22" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="42"/>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="42"/>
+      <c r="AB22" s="42"/>
+      <c r="AC22" s="42"/>
+      <c r="AD22" s="42">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE22" s="42">
+        <f t="shared" si="9"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF22" s="42">
+        <f t="shared" si="9"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG22" s="42">
+        <f t="shared" si="9"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH22" s="42">
+        <f t="shared" si="9"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI22" s="42">
+        <f t="shared" si="9"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ22" s="42">
+        <f t="shared" si="9"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="16">
         <v>21</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="16">
         <v>2</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="17">
         <v>17</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="18">
         <v>0.629</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23" s="18">
         <v>0.28199999999999997</v>
       </c>
-      <c r="J23" s="25">
+      <c r="J23" s="18">
         <v>0.109</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="18">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L23" s="26">
+      <c r="L23" s="19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E24" s="28"/>
-      <c r="F24" s="27"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="35"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="17"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="17"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="17"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="17"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="17"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="17"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="17"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="17"/>
+      <c r="M23" s="43">
+        <f t="shared" si="5"/>
+        <v>5.266</v>
+      </c>
+      <c r="N23" s="42">
+        <f t="shared" si="6"/>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="44"/>
+      <c r="W23" s="44"/>
+      <c r="X23" s="44"/>
+      <c r="Y23" s="44"/>
+      <c r="Z23" s="44"/>
+      <c r="AA23" s="44"/>
+      <c r="AB23" s="44"/>
+      <c r="AC23" s="44"/>
+      <c r="AD23" s="44">
+        <f t="shared" si="9"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE23" s="44">
+        <f t="shared" si="9"/>
+        <v>0.91</v>
+      </c>
+      <c r="AF23" s="44">
+        <f t="shared" si="9"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG23" s="44">
+        <f t="shared" si="9"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH23" s="44">
+        <f t="shared" si="9"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI23" s="44">
+        <f t="shared" si="9"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ23" s="45">
+        <f t="shared" si="9"/>
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B24" s="24">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="42">
+        <v>5.266</v>
+      </c>
+      <c r="N24" s="46">
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="O24" s="42">
+        <v>5.0090000000000003</v>
+      </c>
+      <c r="P24" s="42">
+        <v>4.7409999999999997</v>
+      </c>
+      <c r="Q24" s="42">
+        <v>4.4249999999999998</v>
+      </c>
+      <c r="R24" s="42">
+        <v>4.0910000000000002</v>
+      </c>
+      <c r="S24" s="42">
+        <v>3.68</v>
+      </c>
+      <c r="T24" s="42">
+        <v>3.48</v>
+      </c>
+      <c r="U24" s="42">
+        <v>3.2850000000000001</v>
+      </c>
+      <c r="V24" s="42">
+        <v>3.089</v>
+      </c>
+      <c r="W24" s="42">
+        <v>2.8820000000000001</v>
+      </c>
+      <c r="X24" s="42">
+        <v>2.6960000000000002</v>
+      </c>
+      <c r="Y24" s="42">
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="Z24" s="42">
+        <v>2.077</v>
+      </c>
+      <c r="AA24" s="42">
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="AB24" s="42">
+        <v>1.36</v>
+      </c>
+      <c r="AC24" s="42">
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="AD24" s="42">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AE24" s="42">
+        <v>0.91</v>
+      </c>
+      <c r="AF24" s="42">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="AG24" s="42">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="AH24" s="42">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AI24" s="42">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ24" s="42">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="AK24" s="36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="11"/>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="11"/>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="11"/>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="11"/>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="11"/>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="11"/>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="11"/>
     </row>
     <row r="33" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="17"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="11"/>
     </row>
     <row r="34" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="17"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="11"/>
     </row>
     <row r="35" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="17"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="11"/>
     </row>
     <row r="36" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="17"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="11"/>
     </row>
     <row r="37" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="17"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="11"/>
     </row>
     <row r="38" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="17"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="11"/>
     </row>
     <row r="39" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="17"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="11"/>
     </row>
     <row r="40" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
-      <c r="L40" s="17"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="11"/>
     </row>
     <row r="41" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
-      <c r="L41" s="17"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="11"/>
     </row>
     <row r="42" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="17"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="11"/>
     </row>
     <row r="43" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="17"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="11"/>
     </row>
     <row r="44" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="17"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="AK1:AK2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
constructed rough models of biplane spars with root joint at station 3
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>test #</t>
   </si>
@@ -362,16 +362,32 @@
     <t>MONOPLANE SPAR</t>
   </si>
   <si>
-    <t>BIPLANE SPAR</t>
+    <t>BIPLANE SPAR (15-bispar-rj215-g050)</t>
+  </si>
+  <si>
+    <t>root region</t>
+  </si>
+  <si>
+    <t>root transition region</t>
+  </si>
+  <si>
+    <t>straight biplane region</t>
+  </si>
+  <si>
+    <t>joint transition region</t>
+  </si>
+  <si>
+    <t>outboard monoplane region</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -434,7 +450,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,8 +509,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -878,6 +900,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -886,7 +956,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -998,6 +1068,100 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1028,78 +1192,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1107,17 +1204,6 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
@@ -1141,15 +1227,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>333378</xdr:colOff>
+      <xdr:colOff>752478</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>85723</xdr:rowOff>
+      <xdr:rowOff>171448</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>881285</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>154093</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>166910</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>49318</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1160,7 +1246,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="952503" y="6029323"/>
+          <a:off x="1371603" y="6115048"/>
           <a:ext cx="1509932" cy="1401870"/>
           <a:chOff x="5518209" y="3192216"/>
           <a:chExt cx="3081491" cy="2860960"/>
@@ -3072,15 +3158,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>57159</xdr:rowOff>
+      <xdr:colOff>838199</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38109</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>926627</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>21370</xdr:rowOff>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>2320</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3091,8 +3177,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4324350" y="5619759"/>
-          <a:ext cx="2831627" cy="2059711"/>
+          <a:off x="5095874" y="5791209"/>
+          <a:ext cx="2085975" cy="2059711"/>
           <a:chOff x="922713" y="3325604"/>
           <a:chExt cx="2959331" cy="2942444"/>
         </a:xfrm>
@@ -7252,9 +7338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7275,30 +7361,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="48" t="s">
+      <c r="E1" s="83"/>
+      <c r="F1" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51" t="s">
+      <c r="G1" s="84"/>
+      <c r="H1" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="87"/>
       <c r="M1" s="42" t="s">
         <v>37</v>
       </c>
@@ -7325,17 +7411,17 @@
       <c r="AH1" s="43"/>
       <c r="AI1" s="43"/>
       <c r="AJ1" s="44"/>
-      <c r="AK1" s="47" t="s">
+      <c r="AK1" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="59" t="s">
+      <c r="AL1" s="78" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:38" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="45"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="46"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="80"/>
       <c r="D2" s="22" t="s">
         <v>2</v>
       </c>
@@ -7435,10 +7521,13 @@
       <c r="AJ2" s="26">
         <v>24</v>
       </c>
-      <c r="AK2" s="47"/>
-      <c r="AL2" s="59"/>
+      <c r="AK2" s="81"/>
+      <c r="AL2" s="78"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B3" s="23">
         <v>1</v>
       </c>
@@ -7490,7 +7579,7 @@
         <f>P$24/2</f>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q3" s="56">
+      <c r="Q3" s="46">
         <f>Q$24/2</f>
         <v>2.2124999999999999</v>
       </c>
@@ -7570,7 +7659,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL3" s="70"/>
+      <c r="AL3" s="59"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B4" s="23">
@@ -7624,7 +7713,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q4" s="56">
+      <c r="Q4" s="46">
         <f t="shared" ref="Q4:V19" si="8">Q$24/2</f>
         <v>2.2124999999999999</v>
       </c>
@@ -7704,7 +7793,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL4" s="70"/>
+      <c r="AL4" s="59"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="23">
@@ -7758,7 +7847,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q5" s="56">
+      <c r="Q5" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -7838,7 +7927,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL5" s="70"/>
+      <c r="AL5" s="59"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B6" s="23">
@@ -7892,7 +7981,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q6" s="56">
+      <c r="Q6" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -7972,7 +8061,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL6" s="70"/>
+      <c r="AL6" s="59"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B7" s="23">
@@ -8026,7 +8115,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q7" s="56">
+      <c r="Q7" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -8106,7 +8195,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL7" s="70"/>
+      <c r="AL7" s="59"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B8" s="23">
@@ -8160,7 +8249,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q8" s="56">
+      <c r="Q8" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -8240,7 +8329,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL8" s="70"/>
+      <c r="AL8" s="59"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -8295,7 +8384,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q9" s="57">
+      <c r="Q9" s="47">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -8378,7 +8467,7 @@
       <c r="AK9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AL9" s="71"/>
+      <c r="AL9" s="60"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B10" s="23">
@@ -8420,7 +8509,7 @@
         <f t="shared" si="5"/>
         <v>5.266</v>
       </c>
-      <c r="N10" s="58">
+      <c r="N10" s="48">
         <f t="shared" si="6"/>
         <v>5.2649999999999997</v>
       </c>
@@ -8432,7 +8521,7 @@
         <f>P$24/2</f>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q10" s="56">
+      <c r="Q10" s="46">
         <f>Q$24/2</f>
         <v>2.2124999999999999</v>
       </c>
@@ -8513,7 +8602,7 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="AK10" s="25"/>
-      <c r="AL10" s="70"/>
+      <c r="AL10" s="59"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B11" s="23">
@@ -8567,7 +8656,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q11" s="56">
+      <c r="Q11" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -8647,7 +8736,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL11" s="70"/>
+      <c r="AL11" s="59"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B12" s="23">
@@ -8701,7 +8790,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q12" s="56">
+      <c r="Q12" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -8781,7 +8870,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL12" s="70"/>
+      <c r="AL12" s="59"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B13" s="23">
@@ -8835,7 +8924,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q13" s="56">
+      <c r="Q13" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -8915,7 +9004,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL13" s="70"/>
+      <c r="AL13" s="59"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B14" s="23">
@@ -8969,7 +9058,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q14" s="56">
+      <c r="Q14" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -9049,7 +9138,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL14" s="70"/>
+      <c r="AL14" s="59"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B15" s="23">
@@ -9103,7 +9192,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q15" s="56">
+      <c r="Q15" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -9183,7 +9272,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL15" s="70"/>
+      <c r="AL15" s="59"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
@@ -9196,7 +9285,7 @@
       <c r="D16" s="15">
         <v>2</v>
       </c>
-      <c r="E16" s="55">
+      <c r="E16" s="45">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
@@ -9238,7 +9327,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q16" s="57">
+      <c r="Q16" s="47">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -9318,7 +9407,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL16" s="71"/>
+      <c r="AL16" s="60"/>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -9363,7 +9452,7 @@
         <f t="shared" si="5"/>
         <v>5.266</v>
       </c>
-      <c r="N17" s="58">
+      <c r="N17" s="48">
         <f t="shared" si="6"/>
         <v>5.2649999999999997</v>
       </c>
@@ -9375,7 +9464,7 @@
         <f>P$24/2</f>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q17" s="56">
+      <c r="Q17" s="46">
         <f>Q$24/2</f>
         <v>2.2124999999999999</v>
       </c>
@@ -9456,7 +9545,7 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="AK17" s="25"/>
-      <c r="AL17" s="70"/>
+      <c r="AL17" s="59"/>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B18" s="23">
@@ -9510,7 +9599,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q18" s="56">
+      <c r="Q18" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -9590,7 +9679,7 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL18" s="70"/>
+      <c r="AL18" s="59"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B19" s="23">
@@ -9644,7 +9733,7 @@
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q19" s="56">
+      <c r="Q19" s="46">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
@@ -9677,7 +9766,7 @@
         <v>1.3480000000000001</v>
       </c>
       <c r="Y19" s="35">
-        <f t="shared" ref="Y19:AC23" si="10">Y$24</f>
+        <f t="shared" ref="Y19:AC22" si="10">Y$24</f>
         <v>2.4980000000000002</v>
       </c>
       <c r="Z19" s="34">
@@ -9724,7 +9813,7 @@
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL19" s="70"/>
+      <c r="AL19" s="59"/>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B20" s="23">
@@ -9778,7 +9867,7 @@
         <f t="shared" si="11"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q20" s="56">
+      <c r="Q20" s="46">
         <f t="shared" si="11"/>
         <v>2.2124999999999999</v>
       </c>
@@ -9858,7 +9947,7 @@
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL20" s="70"/>
+      <c r="AL20" s="59"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B21" s="23">
@@ -9912,7 +10001,7 @@
         <f t="shared" si="11"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q21" s="56">
+      <c r="Q21" s="46">
         <f t="shared" si="11"/>
         <v>2.2124999999999999</v>
       </c>
@@ -9992,7 +10081,7 @@
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL21" s="70"/>
+      <c r="AL21" s="59"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B22" s="23">
@@ -10046,7 +10135,7 @@
         <f t="shared" si="11"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q22" s="56">
+      <c r="Q22" s="46">
         <f t="shared" si="11"/>
         <v>2.2124999999999999</v>
       </c>
@@ -10126,7 +10215,7 @@
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL22" s="70"/>
+      <c r="AL22" s="59"/>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
@@ -10181,7 +10270,7 @@
         <f t="shared" si="11"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="Q23" s="57">
+      <c r="Q23" s="47">
         <f t="shared" si="11"/>
         <v>2.2124999999999999</v>
       </c>
@@ -10261,121 +10350,121 @@
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AL23" s="70"/>
+      <c r="AL23" s="59"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="63" t="s">
+      <c r="A24" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="64">
+      <c r="B24" s="53">
         <v>22</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="64" t="s">
+      <c r="D24" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="66" t="s">
+      <c r="E24" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="F24" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="67" t="s">
+      <c r="G24" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="68" t="s">
+      <c r="H24" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="I24" s="68" t="s">
+      <c r="I24" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="J24" s="68" t="s">
+      <c r="J24" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="K24" s="68" t="s">
+      <c r="K24" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="L24" s="69" t="s">
+      <c r="L24" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="M24" s="60">
+      <c r="M24" s="49">
         <v>5.266</v>
       </c>
-      <c r="N24" s="60">
+      <c r="N24" s="49">
         <v>5.2649999999999997</v>
       </c>
-      <c r="O24" s="60">
+      <c r="O24" s="49">
         <v>5.0090000000000003</v>
       </c>
-      <c r="P24" s="60">
+      <c r="P24" s="49">
         <v>4.7409999999999997</v>
       </c>
-      <c r="Q24" s="60">
+      <c r="Q24" s="49">
         <v>4.4249999999999998</v>
       </c>
-      <c r="R24" s="60">
+      <c r="R24" s="49">
         <v>4.0910000000000002</v>
       </c>
-      <c r="S24" s="60">
+      <c r="S24" s="49">
         <v>3.68</v>
       </c>
-      <c r="T24" s="60">
+      <c r="T24" s="49">
         <v>3.48</v>
       </c>
-      <c r="U24" s="60">
+      <c r="U24" s="49">
         <v>3.2850000000000001</v>
       </c>
-      <c r="V24" s="60">
+      <c r="V24" s="49">
         <v>3.089</v>
       </c>
-      <c r="W24" s="60">
+      <c r="W24" s="49">
         <v>2.8820000000000001</v>
       </c>
-      <c r="X24" s="60">
+      <c r="X24" s="49">
         <v>2.6960000000000002</v>
       </c>
-      <c r="Y24" s="60">
+      <c r="Y24" s="49">
         <v>2.4980000000000002</v>
       </c>
-      <c r="Z24" s="60">
+      <c r="Z24" s="49">
         <v>2.077</v>
       </c>
-      <c r="AA24" s="60">
+      <c r="AA24" s="49">
         <v>1.6719999999999999</v>
       </c>
-      <c r="AB24" s="60">
+      <c r="AB24" s="49">
         <v>1.36</v>
       </c>
-      <c r="AC24" s="60">
+      <c r="AC24" s="49">
         <v>1.1379999999999999</v>
       </c>
-      <c r="AD24" s="60">
+      <c r="AD24" s="49">
         <v>0.95399999999999996</v>
       </c>
-      <c r="AE24" s="60">
+      <c r="AE24" s="49">
         <v>0.91</v>
       </c>
-      <c r="AF24" s="60">
+      <c r="AF24" s="49">
         <v>0.83199999999999996</v>
       </c>
-      <c r="AG24" s="60">
+      <c r="AG24" s="49">
         <v>0.79600000000000004</v>
       </c>
-      <c r="AH24" s="60">
+      <c r="AH24" s="49">
         <v>0.70699999999999996</v>
       </c>
-      <c r="AI24" s="60">
+      <c r="AI24" s="49">
         <v>0.65100000000000002</v>
       </c>
-      <c r="AJ24" s="60">
+      <c r="AJ24" s="49">
         <v>0.50800000000000001</v>
       </c>
-      <c r="AK24" s="61" t="s">
+      <c r="AK24" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="AL24" s="62">
+      <c r="AL24" s="51">
         <v>-0.56385624898730002</v>
       </c>
     </row>
@@ -10538,10 +10627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10550,48 +10639,50 @@
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="82" t="s">
+      <c r="C1" s="89"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="83"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="92"/>
     </row>
-    <row r="2" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="s">
+    <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="F2" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="68" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -10601,13 +10692,27 @@
       <c r="C3" s="29">
         <v>6.3E-2</v>
       </c>
-      <c r="D3" s="77">
+      <c r="D3" s="66">
         <f>B3+2*C3</f>
         <v>5.3920000000000003</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="E3" s="29">
+        <f>B3</f>
+        <v>5.266</v>
+      </c>
+      <c r="F3" s="29">
+        <f>C3</f>
+        <v>6.3E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3+2*F3</f>
+        <v>5.3920000000000003</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -10617,13 +10722,30 @@
       <c r="C4" s="29">
         <v>5.5E-2</v>
       </c>
-      <c r="D4" s="77">
+      <c r="D4" s="66">
         <f t="shared" ref="D4:D26" si="0">B4+2*C4</f>
         <v>5.375</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="E4" s="29">
+        <f>B4</f>
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="F4" s="29">
+        <f>C4</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G25" si="1">E4+2*F4</f>
+        <v>5.375</v>
+      </c>
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -10633,13 +10755,27 @@
       <c r="C5" s="29">
         <v>0.04</v>
       </c>
-      <c r="D5" s="77">
+      <c r="D5" s="66">
         <f t="shared" si="0"/>
         <v>5.0890000000000004</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="E5" s="72">
+        <f t="shared" ref="E5:F12" si="2">B5/2</f>
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="F5" s="73">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="G5" s="74">
+        <f t="shared" si="1"/>
+        <v>2.5445000000000002</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -10649,13 +10785,30 @@
       <c r="C6" s="29">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="66">
         <f t="shared" si="0"/>
         <v>4.7909999999999995</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="E6" s="72">
+        <f t="shared" si="2"/>
+        <v>2.3704999999999998</v>
+      </c>
+      <c r="F6" s="73">
+        <f t="shared" si="2"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="G6" s="74">
+        <f t="shared" si="1"/>
+        <v>2.3954999999999997</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -10665,13 +10818,27 @@
       <c r="C7" s="29">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="66">
         <f t="shared" si="0"/>
         <v>4.4550000000000001</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="E7" s="72">
+        <f t="shared" si="2"/>
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="F7" s="73">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G7" s="74">
+        <f t="shared" si="1"/>
+        <v>2.2275</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -10681,13 +10848,27 @@
       <c r="C8" s="29">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="66">
         <f t="shared" si="0"/>
         <v>4.101</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="E8" s="72">
+        <f t="shared" si="2"/>
+        <v>2.0455000000000001</v>
+      </c>
+      <c r="F8" s="73">
+        <f t="shared" si="2"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G8" s="74">
+        <f t="shared" si="1"/>
+        <v>2.0505</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -10697,13 +10878,27 @@
       <c r="C9" s="29">
         <v>0</v>
       </c>
-      <c r="D9" s="77">
+      <c r="D9" s="66">
         <f t="shared" si="0"/>
         <v>3.68</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="E9" s="72">
+        <f t="shared" si="2"/>
+        <v>1.84</v>
+      </c>
+      <c r="F9" s="73">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="74">
+        <f t="shared" si="1"/>
+        <v>1.84</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -10713,13 +10908,27 @@
       <c r="C10" s="29">
         <v>0</v>
       </c>
-      <c r="D10" s="77">
+      <c r="D10" s="66">
         <f t="shared" si="0"/>
         <v>3.48</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="E10" s="72">
+        <f t="shared" si="2"/>
+        <v>1.74</v>
+      </c>
+      <c r="F10" s="73">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="74">
+        <f t="shared" si="1"/>
+        <v>1.74</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -10729,13 +10938,30 @@
       <c r="C11" s="29">
         <v>0</v>
       </c>
-      <c r="D11" s="77">
+      <c r="D11" s="66">
         <f t="shared" si="0"/>
         <v>3.2850000000000001</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="E11" s="72">
+        <f t="shared" si="2"/>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="F11" s="73">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="74">
+        <f t="shared" si="1"/>
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -10745,13 +10971,27 @@
       <c r="C12" s="29">
         <v>0</v>
       </c>
-      <c r="D12" s="77">
+      <c r="D12" s="66">
         <f t="shared" si="0"/>
         <v>3.089</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="E12" s="75">
+        <f t="shared" si="2"/>
+        <v>1.5445</v>
+      </c>
+      <c r="F12" s="76">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="77">
+        <f t="shared" si="1"/>
+        <v>1.5445</v>
+      </c>
+      <c r="I12" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -10761,13 +11001,30 @@
       <c r="C13" s="29">
         <v>0</v>
       </c>
-      <c r="D13" s="77">
+      <c r="D13" s="66">
         <f t="shared" si="0"/>
         <v>2.8820000000000001</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="E13" s="29">
+        <f>B13</f>
+        <v>2.8820000000000001</v>
+      </c>
+      <c r="F13" s="29">
+        <f>C13</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>2.8820000000000001</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -10777,13 +11034,27 @@
       <c r="C14" s="29">
         <v>0</v>
       </c>
-      <c r="D14" s="77">
+      <c r="D14" s="66">
         <f t="shared" si="0"/>
         <v>2.6960000000000002</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="E14" s="29">
+        <f t="shared" ref="E14:E26" si="3">B14</f>
+        <v>2.6960000000000002</v>
+      </c>
+      <c r="F14" s="29">
+        <f t="shared" ref="F14:F25" si="4">C14</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>2.6960000000000002</v>
+      </c>
+      <c r="H14" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -10793,13 +11064,27 @@
       <c r="C15" s="29">
         <v>0</v>
       </c>
-      <c r="D15" s="77">
+      <c r="D15" s="66">
         <f t="shared" si="0"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="E15" s="29">
+        <f t="shared" si="3"/>
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="F15" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="H15" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -10809,13 +11094,27 @@
       <c r="C16" s="29">
         <v>0</v>
       </c>
-      <c r="D16" s="77">
+      <c r="D16" s="66">
         <f t="shared" si="0"/>
         <v>2.077</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="E16" s="29">
+        <f t="shared" si="3"/>
+        <v>2.077</v>
+      </c>
+      <c r="F16" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>2.077</v>
+      </c>
+      <c r="H16" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -10825,13 +11124,27 @@
       <c r="C17" s="29">
         <v>0</v>
       </c>
-      <c r="D17" s="77">
+      <c r="D17" s="66">
         <f t="shared" si="0"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="E17" s="29">
+        <f t="shared" si="3"/>
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="F17" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -10841,13 +11154,27 @@
       <c r="C18" s="29">
         <v>0</v>
       </c>
-      <c r="D18" s="77">
+      <c r="D18" s="66">
         <f t="shared" si="0"/>
         <v>1.36</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="E18" s="29">
+        <f t="shared" si="3"/>
+        <v>1.36</v>
+      </c>
+      <c r="F18" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.36</v>
+      </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -10857,13 +11184,27 @@
       <c r="C19" s="29">
         <v>0</v>
       </c>
-      <c r="D19" s="77">
+      <c r="D19" s="66">
         <f t="shared" si="0"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="G19" s="9"/>
+      <c r="E19" s="29">
+        <f t="shared" si="3"/>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="F19" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -10873,13 +11214,27 @@
       <c r="C20" s="29">
         <v>0</v>
       </c>
-      <c r="D20" s="77">
+      <c r="D20" s="66">
         <f t="shared" si="0"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="G20" s="9"/>
+      <c r="E20" s="29">
+        <f t="shared" si="3"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="F20" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="H20" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -10889,13 +11244,27 @@
       <c r="C21" s="29">
         <v>0</v>
       </c>
-      <c r="D21" s="77">
+      <c r="D21" s="66">
         <f t="shared" si="0"/>
         <v>0.91</v>
       </c>
-      <c r="G21" s="9"/>
+      <c r="E21" s="29">
+        <f t="shared" si="3"/>
+        <v>0.91</v>
+      </c>
+      <c r="F21" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -10905,13 +11274,27 @@
       <c r="C22" s="29">
         <v>0</v>
       </c>
-      <c r="D22" s="77">
+      <c r="D22" s="66">
         <f t="shared" si="0"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="E22" s="29">
+        <f t="shared" si="3"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="F22" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="H22" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -10921,13 +11304,27 @@
       <c r="C23" s="29">
         <v>0</v>
       </c>
-      <c r="D23" s="77">
+      <c r="D23" s="66">
         <f t="shared" si="0"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="G23" s="9"/>
+      <c r="E23" s="29">
+        <f t="shared" si="3"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="F23" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="H23" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -10937,13 +11334,27 @@
       <c r="C24" s="29">
         <v>0</v>
       </c>
-      <c r="D24" s="77">
+      <c r="D24" s="66">
         <f t="shared" si="0"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="G24" s="9"/>
+      <c r="E24" s="29">
+        <f t="shared" si="3"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="F24" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="H24" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -10953,29 +11364,55 @@
       <c r="C25" s="29">
         <v>0</v>
       </c>
-      <c r="D25" s="77">
+      <c r="D25" s="66">
         <f t="shared" si="0"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="G25" s="9"/>
+      <c r="E25" s="29">
+        <f t="shared" si="3"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="F25" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="H25" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="84">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="69">
         <v>24</v>
       </c>
-      <c r="B26" s="85">
+      <c r="B26" s="70">
         <v>0.50800000000000001</v>
       </c>
-      <c r="C26" s="85">
+      <c r="C26" s="70">
         <v>0</v>
       </c>
-      <c r="D26" s="86">
+      <c r="D26" s="71">
         <f t="shared" si="0"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="88"/>
+      <c r="E26" s="70">
+        <f t="shared" si="3"/>
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="F26" s="70">
+        <f>C26</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="69">
+        <f>E26+2*F26</f>
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="H26" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
added @INCLUDE_COMMANDs to DYMORE for extra automation of spar models, with updates to MATLAB and Python scripts
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>test #</t>
   </si>
@@ -378,6 +378,18 @@
   </si>
   <si>
     <t>outboard monoplane region</t>
+  </si>
+  <si>
+    <t>abandoned</t>
+  </si>
+  <si>
+    <t>spar station #11 has curvature k2=0.2011, which gives negative diagonal entries in the stiffness matrix [K]</t>
+  </si>
+  <si>
+    <t>spar station #11 has curvature k2=0.2869, which gives negative diagonal entries in the stiffness matrix [K]</t>
+  </si>
+  <si>
+    <t>spar station #11 has curvature k2=0.2539, which gives negative diagonal entries in the stiffness matrix [K]</t>
   </si>
 </sst>
 </file>
@@ -7340,7 +7352,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7526,7 +7538,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B3" s="23">
         <v>1</v>
@@ -7658,6 +7670,9 @@
       <c r="AJ3" s="30">
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
+      </c>
+      <c r="AK3" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="AL3" s="59"/>
     </row>
@@ -8332,7 +8347,9 @@
       <c r="AL8" s="59"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="B9" s="15">
         <v>7</v>
       </c>
@@ -8470,6 +8487,9 @@
       <c r="AL9" s="60"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="B10" s="23">
         <v>8</v>
       </c>
@@ -8601,7 +8621,9 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AK10" s="25"/>
+      <c r="AK10" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="AL10" s="59"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -9411,7 +9433,7 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B17" s="23">
         <v>15</v>
@@ -9544,7 +9566,9 @@
         <f t="shared" si="2"/>
         <v>0.50800000000000001</v>
       </c>
-      <c r="AK17" s="25"/>
+      <c r="AK17" s="25" t="s">
+        <v>56</v>
+      </c>
       <c r="AL17" s="59"/>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added biplane spar 21, rj=0.629, g=0.50; cleaned up old biplane spar configurations
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="cross-section heights" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="tip deflection results" sheetId="3" r:id="rId2"/>
+    <sheet name="cross-section heights" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
   <si>
     <t>test #</t>
   </si>
@@ -453,6 +453,12 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>rj/R</t>
+  </si>
+  <si>
+    <t>constload tip deflection [m]</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1087,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1385,6 +1391,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="5" builtinId="31"/>
@@ -1475,7 +1490,219 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tip deflection results'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test #</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'tip deflection results'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tip deflection results'!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.4682401240911</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48980424001869999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54492962852030002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56385624898730002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="49972736"/>
+        <c:axId val="49974272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="49972736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49974272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="49974272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.30000000000000004"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>constload tip deflection [m]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49972736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7593,7 +7820,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8578,6 +8805,9 @@
       <c r="AR7" s="55"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B8" s="21">
         <v>6</v>
       </c>
@@ -10878,7 +11108,7 @@
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B23" s="15">
         <v>21</v>
@@ -10931,7 +11161,9 @@
         <f t="shared" si="0"/>
         <v>8.1599999999999999E-4</v>
       </c>
-      <c r="R23" s="14"/>
+      <c r="R23" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="S23" s="29">
         <f t="shared" si="6"/>
         <v>5.266</v>
@@ -11471,6 +11703,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="119" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="119" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="119" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>7</v>
+      </c>
+      <c r="B2" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C2" s="117">
+        <v>1</v>
+      </c>
+      <c r="D2" s="118">
+        <v>0.4682401240911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>14</v>
+      </c>
+      <c r="B3" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C3" s="117">
+        <v>0.75</v>
+      </c>
+      <c r="D3" s="118">
+        <v>0.48980424001869999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>21</v>
+      </c>
+      <c r="B4" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C4" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="118">
+        <v>0.56385624898730002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12267,16 +12589,4 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added biplane spar 6, rj=0.540, g=1.00
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -1528,20 +1528,23 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'tip deflection results'!$A$2:$A$5</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
@@ -1549,20 +1552,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$5</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>0.50663002823820003</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.4682401240911</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1679,7 +1685,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7818,9 +7824,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11703,10 +11709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11730,57 +11736,71 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C2" s="117">
         <v>1</v>
       </c>
       <c r="D2" s="118">
-        <v>0.4682401240911</v>
+        <v>0.50663002823820003</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" s="27">
         <v>0.629</v>
       </c>
       <c r="C3" s="117">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D3" s="118">
-        <v>0.48980424001869999</v>
+        <v>0.4682401240911</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B4" s="27">
         <v>0.629</v>
       </c>
       <c r="C4" s="117">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D4" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.48980424001869999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C5" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="118">
+      <c r="D6" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 13, rj=0.540, g=0.75
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t>test #</t>
   </si>
@@ -1528,10 +1528,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'tip deflection results'!$A$2:$A$6</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -1539,12 +1539,15 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
@@ -1552,10 +1555,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$6</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.50663002823820003</c:v>
                 </c:pt>
@@ -1563,12 +1566,15 @@
                   <c:v>0.4682401240911</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.53227042279350001</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1685,7 +1691,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7826,7 +7832,7 @@
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8812,7 +8818,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B8" s="21">
         <v>6</v>
@@ -9887,6 +9893,9 @@
       <c r="AR14" s="55"/>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B15" s="21">
         <v>13</v>
       </c>
@@ -11709,10 +11718,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11764,43 +11773,57 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C4" s="117">
         <v>0.75</v>
       </c>
       <c r="D4" s="118">
-        <v>0.48980424001869999</v>
+        <v>0.53227042279350001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" s="27">
         <v>0.629</v>
       </c>
       <c r="C5" s="117">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D5" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.48980424001869999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>21</v>
+      </c>
+      <c r="B6" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C6" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="118">
+      <c r="D7" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 20, rj=0.540, g=0.50
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="70">
   <si>
     <t>test #</t>
   </si>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t>constload tip deflection [m]</t>
+  </si>
+  <si>
+    <t>22 (mono)</t>
   </si>
 </sst>
 </file>
@@ -1527,11 +1530,10 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>'tip deflection results'!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+            <c:strRef>
+              <c:f>'tip deflection results'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -1545,20 +1547,23 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
+                <c:pt idx="6">
+                  <c:v>22 (mono)</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$7</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.50663002823820003</c:v>
                 </c:pt>
@@ -1572,9 +1577,12 @@
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.59116965124190002</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1691,7 +1699,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7830,9 +7838,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8664,6 +8672,9 @@
       <c r="AR6" s="55"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B7" s="21">
         <v>5</v>
       </c>
@@ -9894,7 +9905,7 @@
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B15" s="21">
         <v>13</v>
@@ -10969,6 +10980,9 @@
       <c r="AR21" s="55"/>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B22" s="21">
         <v>20</v>
       </c>
@@ -11718,14 +11732,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11801,29 +11816,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C6" s="117">
         <v>0.5</v>
       </c>
       <c r="D6" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.59116965124190002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C7" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="118">
+      <c r="D8" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added spar station 5, rj=0.452, g=1.00
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
   <si>
     <t>test #</t>
   </si>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t>eta</t>
-  </si>
-  <si>
-    <t>in progress</t>
   </si>
   <si>
     <t>rj/R</t>
@@ -1531,28 +1528,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'tip deflection results'!$A$2:$A$8</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>22 (mono)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1560,29 +1560,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$8</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0.55790288509749997</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.50663002823820003</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.4682401240911</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.53227042279350001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.59116965124190002</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1699,7 +1702,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7838,7 +7841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
@@ -8673,7 +8676,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" s="21">
         <v>5</v>
@@ -11732,10 +11735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11749,110 +11752,124 @@
         <v>0</v>
       </c>
       <c r="B1" s="119" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="119" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="119" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C2" s="117">
         <v>1</v>
       </c>
       <c r="D2" s="118">
-        <v>0.50663002823820003</v>
+        <v>0.55790288509749997</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C3" s="117">
         <v>1</v>
       </c>
       <c r="D3" s="118">
-        <v>0.4682401240911</v>
+        <v>0.50663002823820003</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" s="27">
-        <v>0.54</v>
+        <v>0.629</v>
       </c>
       <c r="C4" s="117">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D4" s="118">
-        <v>0.53227042279350001</v>
+        <v>0.4682401240911</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C5" s="117">
         <v>0.75</v>
       </c>
       <c r="D5" s="118">
-        <v>0.48980424001869999</v>
+        <v>0.53227042279350001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B6" s="27">
-        <v>0.54</v>
+        <v>0.629</v>
       </c>
       <c r="C6" s="117">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D6" s="118">
-        <v>0.59116965124190002</v>
+        <v>0.48980424001869999</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C7" s="117">
         <v>0.5</v>
       </c>
       <c r="D7" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.59116965124190002</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="1">
+        <v>21</v>
+      </c>
+      <c r="B8" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C8" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="118">
+      <c r="D9" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 19, rj=0.452, g=0.50
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
   <si>
     <t>test #</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>eta</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
   <si>
     <t>rj/R</t>
@@ -1528,9 +1531,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'tip deflection results'!$A$2:$A$9</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1541,18 +1544,24 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>22 (mono)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1560,10 +1569,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$9</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.55790288509749997</c:v>
                 </c:pt>
@@ -1574,18 +1583,24 @@
                   <c:v>0.4682401240911</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.58425392870920001</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.53227042279350001</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>0.58420106096680002</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.59116965124190002</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1702,7 +1717,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7841,9 +7856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8368,6 +8383,9 @@
       <c r="AR4" s="55"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B5" s="21">
         <v>3</v>
       </c>
@@ -9756,6 +9774,9 @@
       <c r="AR13" s="55"/>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B14" s="21">
         <v>12</v>
       </c>
@@ -9807,7 +9828,9 @@
         <f t="shared" si="0"/>
         <v>1.6616000000000001E-3</v>
       </c>
-      <c r="R14" s="2"/>
+      <c r="R14" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="S14" s="28">
         <f t="shared" si="6"/>
         <v>5.266</v>
@@ -10832,6 +10855,9 @@
       <c r="AR20" s="55"/>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B21" s="21">
         <v>19</v>
       </c>
@@ -10883,7 +10909,9 @@
         <f t="shared" si="0"/>
         <v>1.2461999999999998E-3</v>
       </c>
-      <c r="R21" s="2"/>
+      <c r="R21" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="S21" s="28">
         <f t="shared" si="6"/>
         <v>5.266</v>
@@ -11735,10 +11763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11752,13 +11780,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="119" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" s="119" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="119" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11805,71 +11833,99 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C5" s="117">
         <v>0.75</v>
       </c>
       <c r="D5" s="118">
-        <v>0.53227042279350001</v>
+        <v>0.58425392870920001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C6" s="117">
         <v>0.75</v>
       </c>
       <c r="D6" s="118">
-        <v>0.48980424001869999</v>
+        <v>0.53227042279350001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" s="27">
-        <v>0.54</v>
+        <v>0.629</v>
       </c>
       <c r="C7" s="117">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D7" s="118">
-        <v>0.59116965124190002</v>
+        <v>0.48980424001869999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="27">
-        <v>0.629</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C8" s="117">
         <v>0.5</v>
       </c>
       <c r="D8" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.58420106096680002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="1">
+        <v>20</v>
+      </c>
+      <c r="B9" s="27">
+        <v>0.54</v>
+      </c>
+      <c r="C9" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="118">
+        <v>0.59116965124190002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>21</v>
+      </c>
+      <c r="B10" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C10" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="118">
+      <c r="D11" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 3, rj=0.274, g=1.00
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="70">
   <si>
     <t>test #</t>
   </si>
@@ -1531,37 +1531,40 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'tip deflection results'!$A$2:$A$11</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>22 (mono)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1569,38 +1572,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$11</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>0.68802083102529998</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.55790288509749997</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.50663002823820003</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.4682401240911</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.58425392870920001</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.53227042279350001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.58420106096680002</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.59116965124190002</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1660,7 +1666,7 @@
         <c:axId val="49974272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.30000000000000004"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1717,7 +1723,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7858,7 +7864,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8384,7 +8390,7 @@
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" s="21">
         <v>3</v>
@@ -9472,6 +9478,9 @@
       <c r="AR11" s="55"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B12" s="21">
         <v>10</v>
       </c>
@@ -9625,6 +9634,9 @@
       <c r="AR12" s="55"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="B13" s="85">
         <v>11</v>
       </c>
@@ -11763,10 +11775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11791,141 +11803,155 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C2" s="117">
         <v>1</v>
       </c>
       <c r="D2" s="118">
-        <v>0.55790288509749997</v>
+        <v>0.68802083102529998</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C3" s="117">
         <v>1</v>
       </c>
       <c r="D3" s="118">
-        <v>0.50663002823820003</v>
+        <v>0.55790288509749997</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C4" s="117">
         <v>1</v>
       </c>
       <c r="D4" s="118">
-        <v>0.4682401240911</v>
+        <v>0.50663002823820003</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.629</v>
       </c>
       <c r="C5" s="117">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D5" s="118">
-        <v>0.58425392870920001</v>
+        <v>0.4682401240911</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C6" s="117">
         <v>0.75</v>
       </c>
       <c r="D6" s="118">
-        <v>0.53227042279350001</v>
+        <v>0.58425392870920001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C7" s="117">
         <v>0.75</v>
       </c>
       <c r="D7" s="118">
-        <v>0.48980424001869999</v>
+        <v>0.53227042279350001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.629</v>
       </c>
       <c r="C8" s="117">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D8" s="118">
-        <v>0.58420106096680002</v>
+        <v>0.48980424001869999</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C9" s="117">
         <v>0.5</v>
       </c>
       <c r="D9" s="118">
-        <v>0.59116965124190002</v>
+        <v>0.58420106096680002</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C10" s="117">
         <v>0.5</v>
       </c>
       <c r="D10" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.59116965124190002</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="1">
+        <v>21</v>
+      </c>
+      <c r="B11" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C11" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D12" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 10, rj=0.274, g=0.75
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="70">
   <si>
     <t>test #</t>
   </si>
@@ -1531,9 +1531,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'tip deflection results'!$A$2:$A$12</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1547,24 +1547,27 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>22 (mono)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1572,10 +1575,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$12</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.68802083102529998</c:v>
                 </c:pt>
@@ -1589,24 +1592,27 @@
                   <c:v>0.4682401240911</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.70512802088869997</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.58425392870920001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.53227042279350001</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.58420106096680002</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.59116965124190002</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1723,7 +1729,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7864,7 +7870,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9479,7 +9485,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B12" s="21">
         <v>10</v>
@@ -10562,6 +10568,9 @@
       <c r="AR18" s="55"/>
     </row>
     <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B19" s="21">
         <v>17</v>
       </c>
@@ -11775,10 +11784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11859,99 +11868,113 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C6" s="117">
         <v>0.75</v>
       </c>
       <c r="D6" s="118">
-        <v>0.58425392870920001</v>
+        <v>0.70512802088869997</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C7" s="117">
         <v>0.75</v>
       </c>
       <c r="D7" s="118">
-        <v>0.53227042279350001</v>
+        <v>0.58425392870920001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C8" s="117">
         <v>0.75</v>
       </c>
       <c r="D8" s="118">
-        <v>0.48980424001869999</v>
+        <v>0.53227042279350001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B9" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.629</v>
       </c>
       <c r="C9" s="117">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D9" s="118">
-        <v>0.58420106096680002</v>
+        <v>0.48980424001869999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C10" s="117">
         <v>0.5</v>
       </c>
       <c r="D10" s="118">
-        <v>0.59116965124190002</v>
+        <v>0.58420106096680002</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C11" s="117">
         <v>0.5</v>
       </c>
       <c r="D11" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.59116965124190002</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="1">
+        <v>21</v>
+      </c>
+      <c r="B12" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C12" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="118">
+      <c r="D13" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 17, rj=0.274, g=0.50
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
   <si>
     <t>test #</t>
   </si>
@@ -1531,9 +1531,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'tip deflection results'!$A$2:$A$13</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$14</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1559,15 +1559,18 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>22 (mono)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1575,10 +1578,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$13</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.68802083102529998</c:v>
                 </c:pt>
@@ -1604,15 +1607,18 @@
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.7331210458563</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.58420106096680002</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.59116965124190002</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1729,7 +1735,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7868,9 +7874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8242,6 +8248,9 @@
       <c r="AR3" s="55"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B4" s="21">
         <v>2</v>
       </c>
@@ -10569,7 +10578,7 @@
     </row>
     <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="21">
         <v>17</v>
@@ -11784,10 +11793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11924,57 +11933,71 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C10" s="117">
         <v>0.5</v>
       </c>
       <c r="D10" s="118">
-        <v>0.58420106096680002</v>
+        <v>0.7331210458563</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C11" s="117">
         <v>0.5</v>
       </c>
       <c r="D11" s="118">
-        <v>0.59116965124190002</v>
+        <v>0.58420106096680002</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C12" s="117">
         <v>0.5</v>
       </c>
       <c r="D12" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.59116965124190002</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="1">
+        <v>21</v>
+      </c>
+      <c r="B13" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C13" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="118">
+      <c r="D14" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 2, rj=0.245, g=1.00
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
   <si>
     <t>test #</t>
   </si>
@@ -1531,46 +1531,49 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'tip deflection results'!$A$2:$A$14</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>22 (mono)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1578,47 +1581,50 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$14</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0.69280723872630001</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.68802083102529998</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.55790288509749997</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.50663002823820003</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4682401240911</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.70512802088869997</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.58425392870920001</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.53227042279350001</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.7331210458563</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.58420106096680002</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.59116965124190002</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1733,10 +1739,10 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7876,7 +7882,7 @@
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8249,7 +8255,7 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="21">
         <v>2</v>
@@ -9340,6 +9346,9 @@
       <c r="AR10" s="55"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B11" s="21">
         <v>9</v>
       </c>
@@ -11793,10 +11802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11821,183 +11830,197 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="27">
-        <v>0.27400000000000002</v>
+        <v>0.245</v>
       </c>
       <c r="C2" s="117">
         <v>1</v>
       </c>
       <c r="D2" s="118">
-        <v>0.68802083102529998</v>
+        <v>0.69280723872630001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C3" s="117">
         <v>1</v>
       </c>
       <c r="D3" s="118">
-        <v>0.55790288509749997</v>
+        <v>0.68802083102529998</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C4" s="117">
         <v>1</v>
       </c>
       <c r="D4" s="118">
-        <v>0.50663002823820003</v>
+        <v>0.55790288509749997</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C5" s="117">
         <v>1</v>
       </c>
       <c r="D5" s="118">
-        <v>0.4682401240911</v>
+        <v>0.50663002823820003</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="27">
-        <v>0.27400000000000002</v>
+        <v>0.629</v>
       </c>
       <c r="C6" s="117">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D6" s="118">
-        <v>0.70512802088869997</v>
+        <v>0.4682401240911</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C7" s="117">
         <v>0.75</v>
       </c>
       <c r="D7" s="118">
-        <v>0.58425392870920001</v>
+        <v>0.70512802088869997</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C8" s="117">
         <v>0.75</v>
       </c>
       <c r="D8" s="118">
-        <v>0.53227042279350001</v>
+        <v>0.58425392870920001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C9" s="117">
         <v>0.75</v>
       </c>
       <c r="D9" s="118">
-        <v>0.48980424001869999</v>
+        <v>0.53227042279350001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="27">
-        <v>0.27400000000000002</v>
+        <v>0.629</v>
       </c>
       <c r="C10" s="117">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D10" s="118">
-        <v>0.7331210458563</v>
+        <v>0.48980424001869999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C11" s="117">
         <v>0.5</v>
       </c>
       <c r="D11" s="118">
-        <v>0.58420106096680002</v>
+        <v>0.7331210458563</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C12" s="117">
         <v>0.5</v>
       </c>
       <c r="D12" s="118">
-        <v>0.59116965124190002</v>
+        <v>0.58420106096680002</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C13" s="117">
         <v>0.5</v>
       </c>
       <c r="D13" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.59116965124190002</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="1">
+        <v>21</v>
+      </c>
+      <c r="B14" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C14" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="118">
+      <c r="D15" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 9, rj=0.245, g=0.75
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
   <si>
     <t>test #</t>
   </si>
@@ -1531,9 +1531,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'tip deflection results'!$A$2:$A$15</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1550,30 +1550,33 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>22 (mono)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1581,10 +1584,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$15</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0.69280723872630001</c:v>
                 </c:pt>
@@ -1601,30 +1604,33 @@
                   <c:v>0.4682401240911</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.70697489391379997</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.70512802088869997</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.58425392870920001</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.53227042279350001</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.7331210458563</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.58420106096680002</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.59116965124190002</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1741,7 +1747,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7882,7 +7888,7 @@
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9347,7 +9353,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="21">
         <v>9</v>
@@ -10433,6 +10439,9 @@
       <c r="AR17" s="55"/>
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B18" s="21">
         <v>16</v>
       </c>
@@ -11802,10 +11811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11900,127 +11909,141 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="27">
-        <v>0.27400000000000002</v>
+        <v>0.245</v>
       </c>
       <c r="C7" s="117">
         <v>0.75</v>
       </c>
       <c r="D7" s="118">
-        <v>0.70512802088869997</v>
+        <v>0.70697489391379997</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C8" s="117">
         <v>0.75</v>
       </c>
       <c r="D8" s="118">
-        <v>0.58425392870920001</v>
+        <v>0.70512802088869997</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C9" s="117">
         <v>0.75</v>
       </c>
       <c r="D9" s="118">
-        <v>0.53227042279350001</v>
+        <v>0.58425392870920001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C10" s="117">
         <v>0.75</v>
       </c>
       <c r="D10" s="118">
-        <v>0.48980424001869999</v>
+        <v>0.53227042279350001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="27">
-        <v>0.27400000000000002</v>
+        <v>0.629</v>
       </c>
       <c r="C11" s="117">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D11" s="118">
-        <v>0.7331210458563</v>
+        <v>0.48980424001869999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C12" s="117">
         <v>0.5</v>
       </c>
       <c r="D12" s="118">
-        <v>0.58420106096680002</v>
+        <v>0.7331210458563</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C13" s="117">
         <v>0.5</v>
       </c>
       <c r="D13" s="118">
-        <v>0.59116965124190002</v>
+        <v>0.58420106096680002</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C14" s="117">
         <v>0.5</v>
       </c>
       <c r="D14" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.59116965124190002</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="1">
+        <v>21</v>
+      </c>
+      <c r="B15" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C15" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="118">
+      <c r="D16" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added biplane spar 16, rj=0.245, g=0.50; finished all constload cases
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="69">
   <si>
     <t>test #</t>
   </si>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t>eta</t>
-  </si>
-  <si>
-    <t>in progress</t>
   </si>
   <si>
     <t>rj/R</t>
@@ -1531,9 +1528,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'tip deflection results'!$A$2:$A$16</c:f>
+              <c:f>'tip deflection results'!$A$2:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1565,18 +1562,21 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>22 (mono)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1584,10 +1584,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tip deflection results'!$D$2:$D$16</c:f>
+              <c:f>'tip deflection results'!$D$2:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.69280723872630001</c:v>
                 </c:pt>
@@ -1619,18 +1619,21 @@
                   <c:v>0.48980424001869999</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0.73025348365450005</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.7331210458563</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.58420106096680002</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.59116965124190002</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.54492962852030002</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.56385624898730002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1747,7 +1750,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7886,7 +7889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
@@ -10440,7 +10443,7 @@
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" s="21">
         <v>16</v>
@@ -11811,10 +11814,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11828,13 +11831,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="119" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="119" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="119" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11979,71 +11982,85 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="27">
-        <v>0.27400000000000002</v>
+        <v>0.245</v>
       </c>
       <c r="C12" s="117">
         <v>0.5</v>
       </c>
       <c r="D12" s="118">
-        <v>0.7331210458563</v>
+        <v>0.73025348365450005</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="27">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C13" s="117">
         <v>0.5</v>
       </c>
       <c r="D13" s="118">
-        <v>0.58420106096680002</v>
+        <v>0.7331210458563</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="27">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C14" s="117">
         <v>0.5</v>
       </c>
       <c r="D14" s="118">
-        <v>0.59116965124190002</v>
+        <v>0.58420106096680002</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="27">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C15" s="117">
         <v>0.5</v>
       </c>
       <c r="D15" s="118">
-        <v>0.54492962852030002</v>
+        <v>0.59116965124190002</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="1">
+        <v>21</v>
+      </c>
+      <c r="B16" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="C16" s="117">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="118">
+        <v>0.54492962852030002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="118">
+      <c r="D17" s="118">
         <v>0.56385624898730002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started postprocessing DYMORE results
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,8 +553,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +630,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1079,15 +1091,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1327,6 +1340,28 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1378,35 +1413,17 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="40% - Accent1" xfId="5" builtinId="31"/>
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -1649,11 +1666,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="49972736"/>
-        <c:axId val="49974272"/>
+        <c:axId val="106637568"/>
+        <c:axId val="106668416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49972736"/>
+        <c:axId val="106637568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1682,7 +1699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49974272"/>
+        <c:crossAx val="106668416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1690,7 +1707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49974272"/>
+        <c:axId val="106668416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.4"/>
@@ -1721,7 +1738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49972736"/>
+        <c:crossAx val="106637568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7889,7 +7906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
@@ -7916,38 +7933,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="100"/>
-      <c r="F1" s="99" t="s">
+      <c r="E1" s="108"/>
+      <c r="F1" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="101"/>
-      <c r="H1" s="102" t="s">
+      <c r="G1" s="109"/>
+      <c r="H1" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="106" t="s">
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="114" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="104"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="112"/>
       <c r="S1" s="77" t="s">
         <v>36</v>
       </c>
@@ -7974,17 +7991,17 @@
       <c r="AN1" s="39"/>
       <c r="AO1" s="39"/>
       <c r="AP1" s="40"/>
-      <c r="AQ1" s="98" t="s">
+      <c r="AQ1" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="AR1" s="95" t="s">
+      <c r="AR1" s="103" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:44" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="96"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="97"/>
+      <c r="A2" s="104"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
@@ -8102,8 +8119,8 @@
       <c r="AP2" s="24">
         <v>24</v>
       </c>
-      <c r="AQ2" s="98"/>
-      <c r="AR2" s="95"/>
+      <c r="AQ2" s="106"/>
+      <c r="AR2" s="103"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -8144,17 +8161,17 @@
       <c r="L3" s="91">
         <v>1</v>
       </c>
-      <c r="M3" s="114">
+      <c r="M3" s="97">
         <v>10</v>
       </c>
-      <c r="N3" s="115"/>
-      <c r="O3" s="116">
+      <c r="N3" s="98"/>
+      <c r="O3" s="99">
         <v>1.5445</v>
       </c>
-      <c r="P3" s="116">
+      <c r="P3" s="99">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="Q3" s="116">
+      <c r="Q3" s="99">
         <f t="shared" ref="Q3:Q23" si="0">O3*P3</f>
         <v>3.5214599999999999E-2</v>
       </c>
@@ -8304,7 +8321,7 @@
       <c r="M4" s="79">
         <v>11</v>
       </c>
-      <c r="N4" s="112">
+      <c r="N4" s="95">
         <v>0.5</v>
       </c>
       <c r="O4" s="81">
@@ -8460,7 +8477,7 @@
       <c r="M5" s="79">
         <v>12</v>
       </c>
-      <c r="N5" s="112">
+      <c r="N5" s="95">
         <v>0.5</v>
       </c>
       <c r="O5" s="81">
@@ -8613,17 +8630,17 @@
       <c r="L6" s="91">
         <v>1</v>
       </c>
-      <c r="M6" s="114">
+      <c r="M6" s="97">
         <v>13</v>
       </c>
-      <c r="N6" s="115"/>
-      <c r="O6" s="116">
+      <c r="N6" s="98"/>
+      <c r="O6" s="99">
         <v>1.2490000000000001</v>
       </c>
-      <c r="P6" s="116">
+      <c r="P6" s="99">
         <v>4.1599999999999998E-2</v>
       </c>
-      <c r="Q6" s="116">
+      <c r="Q6" s="99">
         <f t="shared" si="0"/>
         <v>5.1958400000000002E-2</v>
       </c>
@@ -8770,7 +8787,7 @@
       <c r="M7" s="79">
         <v>14</v>
       </c>
-      <c r="N7" s="112">
+      <c r="N7" s="95">
         <v>0.50409999999999999</v>
       </c>
       <c r="O7" s="81">
@@ -8926,7 +8943,7 @@
       <c r="M8" s="79">
         <v>15</v>
       </c>
-      <c r="N8" s="112">
+      <c r="N8" s="95">
         <v>0.5</v>
       </c>
       <c r="O8" s="81">
@@ -9082,7 +9099,7 @@
       <c r="M9" s="80">
         <v>16</v>
       </c>
-      <c r="N9" s="113">
+      <c r="N9" s="96">
         <v>0.49590000000000001</v>
       </c>
       <c r="O9" s="82">
@@ -9238,17 +9255,17 @@
       <c r="L10" s="91">
         <v>0.75</v>
       </c>
-      <c r="M10" s="114">
+      <c r="M10" s="97">
         <v>10</v>
       </c>
-      <c r="N10" s="115"/>
-      <c r="O10" s="116">
+      <c r="N10" s="98"/>
+      <c r="O10" s="99">
         <v>1.5445</v>
       </c>
-      <c r="P10" s="116">
+      <c r="P10" s="99">
         <v>0.25390000000000001</v>
       </c>
-      <c r="Q10" s="116">
+      <c r="Q10" s="99">
         <f t="shared" si="0"/>
         <v>0.39214855000000004</v>
       </c>
@@ -9396,7 +9413,7 @@
       <c r="M11" s="79">
         <v>11</v>
       </c>
-      <c r="N11" s="112">
+      <c r="N11" s="95">
         <v>0.5</v>
       </c>
       <c r="O11" s="81">
@@ -9552,7 +9569,7 @@
       <c r="M12" s="79">
         <v>12</v>
       </c>
-      <c r="N12" s="112">
+      <c r="N12" s="95">
         <v>0.5</v>
       </c>
       <c r="O12" s="81">
@@ -9705,17 +9722,17 @@
       <c r="L13" s="91">
         <v>0.75</v>
       </c>
-      <c r="M13" s="114">
+      <c r="M13" s="97">
         <v>13</v>
       </c>
-      <c r="N13" s="115"/>
-      <c r="O13" s="116">
+      <c r="N13" s="98"/>
+      <c r="O13" s="99">
         <v>1.2490000000000001</v>
       </c>
-      <c r="P13" s="116">
+      <c r="P13" s="99">
         <v>0.11210000000000001</v>
       </c>
-      <c r="Q13" s="116">
+      <c r="Q13" s="99">
         <f t="shared" si="0"/>
         <v>0.14001290000000002</v>
       </c>
@@ -9860,7 +9877,7 @@
       <c r="M14" s="79">
         <v>14</v>
       </c>
-      <c r="N14" s="112">
+      <c r="N14" s="95">
         <v>0.50409999999999999</v>
       </c>
       <c r="O14" s="81">
@@ -10016,7 +10033,7 @@
       <c r="M15" s="79">
         <v>15</v>
       </c>
-      <c r="N15" s="112">
+      <c r="N15" s="95">
         <v>0.5</v>
       </c>
       <c r="O15" s="81">
@@ -10172,7 +10189,7 @@
       <c r="M16" s="80">
         <v>16</v>
       </c>
-      <c r="N16" s="113">
+      <c r="N16" s="96">
         <v>0.49590000000000001</v>
       </c>
       <c r="O16" s="82">
@@ -10325,17 +10342,17 @@
       <c r="L17" s="91">
         <v>0.5</v>
       </c>
-      <c r="M17" s="114">
+      <c r="M17" s="97">
         <v>10</v>
       </c>
-      <c r="N17" s="115"/>
-      <c r="O17" s="116">
+      <c r="N17" s="98"/>
+      <c r="O17" s="99">
         <v>1.5445</v>
       </c>
-      <c r="P17" s="116">
+      <c r="P17" s="99">
         <v>0.28689999999999999</v>
       </c>
-      <c r="Q17" s="116">
+      <c r="Q17" s="99">
         <f t="shared" si="0"/>
         <v>0.44311704999999996</v>
       </c>
@@ -10483,7 +10500,7 @@
       <c r="M18" s="79">
         <v>11</v>
       </c>
-      <c r="N18" s="112">
+      <c r="N18" s="95">
         <v>0.5</v>
       </c>
       <c r="O18" s="81">
@@ -10639,7 +10656,7 @@
       <c r="M19" s="79">
         <v>12</v>
       </c>
-      <c r="N19" s="112">
+      <c r="N19" s="95">
         <v>0.5</v>
       </c>
       <c r="O19" s="81">
@@ -10792,17 +10809,17 @@
       <c r="L20" s="91">
         <v>0.5</v>
       </c>
-      <c r="M20" s="114">
+      <c r="M20" s="97">
         <v>13</v>
       </c>
-      <c r="N20" s="115"/>
-      <c r="O20" s="116">
+      <c r="N20" s="98"/>
+      <c r="O20" s="99">
         <v>1.2490000000000001</v>
       </c>
-      <c r="P20" s="116">
+      <c r="P20" s="99">
         <v>7.8399999999999997E-2</v>
       </c>
-      <c r="Q20" s="116">
+      <c r="Q20" s="99">
         <f t="shared" si="0"/>
         <v>9.7921600000000011E-2</v>
       </c>
@@ -10947,7 +10964,7 @@
       <c r="M21" s="79">
         <v>14</v>
       </c>
-      <c r="N21" s="112">
+      <c r="N21" s="95">
         <v>0.50409999999999999</v>
       </c>
       <c r="O21" s="81">
@@ -11103,7 +11120,7 @@
       <c r="M22" s="79">
         <v>15</v>
       </c>
-      <c r="N22" s="112">
+      <c r="N22" s="95">
         <v>0.5</v>
       </c>
       <c r="O22" s="81">
@@ -11259,7 +11276,7 @@
       <c r="M23" s="80">
         <v>16</v>
       </c>
-      <c r="N23" s="113">
+      <c r="N23" s="96">
         <v>0.49590000000000001</v>
       </c>
       <c r="O23" s="82">
@@ -11816,8 +11833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11827,16 +11844,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="C1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="119" t="s">
+      <c r="D1" s="102" t="s">
         <v>67</v>
       </c>
     </row>
@@ -11847,10 +11864,10 @@
       <c r="B2" s="27">
         <v>0.245</v>
       </c>
-      <c r="C2" s="117">
+      <c r="C2" s="100">
         <v>1</v>
       </c>
-      <c r="D2" s="118">
+      <c r="D2" s="101">
         <v>0.69280723872630001</v>
       </c>
     </row>
@@ -11861,10 +11878,10 @@
       <c r="B3" s="27">
         <v>0.27400000000000002</v>
       </c>
-      <c r="C3" s="117">
+      <c r="C3" s="100">
         <v>1</v>
       </c>
-      <c r="D3" s="118">
+      <c r="D3" s="101">
         <v>0.68802083102529998</v>
       </c>
     </row>
@@ -11875,10 +11892,10 @@
       <c r="B4" s="27">
         <v>0.45200000000000001</v>
       </c>
-      <c r="C4" s="117">
+      <c r="C4" s="100">
         <v>1</v>
       </c>
-      <c r="D4" s="118">
+      <c r="D4" s="101">
         <v>0.55790288509749997</v>
       </c>
     </row>
@@ -11889,24 +11906,24 @@
       <c r="B5" s="27">
         <v>0.54</v>
       </c>
-      <c r="C5" s="117">
+      <c r="C5" s="100">
         <v>1</v>
       </c>
-      <c r="D5" s="118">
+      <c r="D5" s="101">
         <v>0.50663002823820003</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="120">
         <v>7</v>
       </c>
       <c r="B6" s="27">
         <v>0.629</v>
       </c>
-      <c r="C6" s="117">
+      <c r="C6" s="100">
         <v>1</v>
       </c>
-      <c r="D6" s="118">
+      <c r="D6" s="101">
         <v>0.4682401240911</v>
       </c>
     </row>
@@ -11917,10 +11934,10 @@
       <c r="B7" s="27">
         <v>0.245</v>
       </c>
-      <c r="C7" s="117">
+      <c r="C7" s="100">
         <v>0.75</v>
       </c>
-      <c r="D7" s="118">
+      <c r="D7" s="101">
         <v>0.70697489391379997</v>
       </c>
     </row>
@@ -11931,10 +11948,10 @@
       <c r="B8" s="27">
         <v>0.27400000000000002</v>
       </c>
-      <c r="C8" s="117">
+      <c r="C8" s="100">
         <v>0.75</v>
       </c>
-      <c r="D8" s="118">
+      <c r="D8" s="101">
         <v>0.70512802088869997</v>
       </c>
     </row>
@@ -11945,10 +11962,10 @@
       <c r="B9" s="27">
         <v>0.45200000000000001</v>
       </c>
-      <c r="C9" s="117">
+      <c r="C9" s="100">
         <v>0.75</v>
       </c>
-      <c r="D9" s="118">
+      <c r="D9" s="101">
         <v>0.58425392870920001</v>
       </c>
     </row>
@@ -11959,24 +11976,24 @@
       <c r="B10" s="27">
         <v>0.54</v>
       </c>
-      <c r="C10" s="117">
+      <c r="C10" s="100">
         <v>0.75</v>
       </c>
-      <c r="D10" s="118">
+      <c r="D10" s="101">
         <v>0.53227042279350001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="120">
         <v>14</v>
       </c>
       <c r="B11" s="27">
         <v>0.629</v>
       </c>
-      <c r="C11" s="117">
+      <c r="C11" s="100">
         <v>0.75</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D11" s="101">
         <v>0.48980424001869999</v>
       </c>
     </row>
@@ -11987,10 +12004,10 @@
       <c r="B12" s="27">
         <v>0.245</v>
       </c>
-      <c r="C12" s="117">
+      <c r="C12" s="100">
         <v>0.5</v>
       </c>
-      <c r="D12" s="118">
+      <c r="D12" s="101">
         <v>0.73025348365450005</v>
       </c>
     </row>
@@ -12001,10 +12018,10 @@
       <c r="B13" s="27">
         <v>0.27400000000000002</v>
       </c>
-      <c r="C13" s="117">
+      <c r="C13" s="100">
         <v>0.5</v>
       </c>
-      <c r="D13" s="118">
+      <c r="D13" s="101">
         <v>0.7331210458563</v>
       </c>
     </row>
@@ -12015,10 +12032,10 @@
       <c r="B14" s="27">
         <v>0.45200000000000001</v>
       </c>
-      <c r="C14" s="117">
+      <c r="C14" s="100">
         <v>0.5</v>
       </c>
-      <c r="D14" s="118">
+      <c r="D14" s="101">
         <v>0.58420106096680002</v>
       </c>
     </row>
@@ -12029,10 +12046,10 @@
       <c r="B15" s="27">
         <v>0.54</v>
       </c>
-      <c r="C15" s="117">
+      <c r="C15" s="100">
         <v>0.5</v>
       </c>
-      <c r="D15" s="118">
+      <c r="D15" s="101">
         <v>0.59116965124190002</v>
       </c>
     </row>
@@ -12043,10 +12060,10 @@
       <c r="B16" s="27">
         <v>0.629</v>
       </c>
-      <c r="C16" s="117">
+      <c r="C16" s="100">
         <v>0.5</v>
       </c>
-      <c r="D16" s="118">
+      <c r="D16" s="101">
         <v>0.54492962852030002</v>
       </c>
     </row>
@@ -12060,7 +12077,7 @@
       <c r="C17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="118">
+      <c r="D17" s="101">
         <v>0.56385624898730002</v>
       </c>
     </row>
@@ -12094,16 +12111,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="108"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="110" t="s">
+      <c r="C1" s="116"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="110"/>
-      <c r="G1" s="111"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="119"/>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">

</xml_diff>

<commit_message>
made contour plot of parametric sweep
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
@@ -1362,6 +1362,9 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1412,9 +1415,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1666,11 +1666,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="106637568"/>
-        <c:axId val="106668416"/>
+        <c:axId val="103033088"/>
+        <c:axId val="103068032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="106637568"/>
+        <c:axId val="103033088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1699,7 +1699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106668416"/>
+        <c:crossAx val="103068032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1707,7 +1707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106668416"/>
+        <c:axId val="103068032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.4"/>
@@ -1738,7 +1738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106637568"/>
+        <c:crossAx val="103033088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7933,38 +7933,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="105" t="s">
+      <c r="C1" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="D1" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="108"/>
-      <c r="F1" s="107" t="s">
+      <c r="E1" s="109"/>
+      <c r="F1" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="109"/>
-      <c r="H1" s="110" t="s">
+      <c r="G1" s="110"/>
+      <c r="H1" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="114" t="s">
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="113"/>
       <c r="S1" s="77" t="s">
         <v>36</v>
       </c>
@@ -7991,17 +7991,17 @@
       <c r="AN1" s="39"/>
       <c r="AO1" s="39"/>
       <c r="AP1" s="40"/>
-      <c r="AQ1" s="106" t="s">
+      <c r="AQ1" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="AR1" s="103" t="s">
+      <c r="AR1" s="104" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:44" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="104"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="105"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="106"/>
       <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
@@ -8119,8 +8119,8 @@
       <c r="AP2" s="24">
         <v>24</v>
       </c>
-      <c r="AQ2" s="106"/>
-      <c r="AR2" s="103"/>
+      <c r="AQ2" s="107"/>
+      <c r="AR2" s="104"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -11834,7 +11834,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11914,7 +11914,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="120">
+      <c r="A6" s="103">
         <v>7</v>
       </c>
       <c r="B6" s="27">
@@ -11984,7 +11984,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="120">
+      <c r="A11" s="103">
         <v>14</v>
       </c>
       <c r="B11" s="27">
@@ -12111,16 +12111,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="118" t="s">
+      <c r="C1" s="117"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="118"/>
-      <c r="G1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="120"/>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">

</xml_diff>

<commit_message>
made a toggle for the root joint throughout spardesign
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
   <si>
     <t>test #</t>
   </si>
@@ -1566,11 +1566,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101132544"/>
-        <c:axId val="101171584"/>
+        <c:axId val="103897344"/>
+        <c:axId val="103920000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101132544"/>
+        <c:axId val="103897344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1598,7 +1598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101171584"/>
+        <c:crossAx val="103920000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1606,7 +1606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101171584"/>
+        <c:axId val="103920000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.4"/>
@@ -1636,7 +1636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101132544"/>
+        <c:crossAx val="103897344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9190,6 +9190,9 @@
       <c r="AP10" s="46"/>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="B11" s="18">
         <v>9</v>
       </c>
@@ -11502,7 +11505,7 @@
       <formula>NOT(ISERROR(SEARCH("NO",P3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A24">
+  <conditionalFormatting sqref="A19:A24 A3:A17">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="completed">
       <formula>NOT(ISERROR(SEARCH("completed",A3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
started plotting new results for full-hSW bispars
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
@@ -349,9 +349,6 @@
     <t>constload tip deflection [m]</t>
   </si>
   <si>
-    <t>22 (mono)</t>
-  </si>
-  <si>
     <t>completed</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>dimless params</t>
+  </si>
+  <si>
+    <t>0 (mono)</t>
   </si>
 </sst>
 </file>
@@ -1249,54 +1249,6 @@
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1373,6 +1325,54 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1508,52 +1508,52 @@
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>0 (mono)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>17</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22 (mono)</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1565,52 +1565,52 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.69280723872630001</c:v>
+                  <c:v>0.56385624898730002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.68802083102529998</c:v>
+                  <c:v>0.50484503415899995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55790288509749997</c:v>
+                  <c:v>0.49601387384309997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.50663002823820003</c:v>
+                  <c:v>0.39042208149230001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4682401240911</c:v>
+                  <c:v>0.33874927541130001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.70697489391379997</c:v>
+                  <c:v>0.28565397168509998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70512802088869997</c:v>
+                  <c:v>0.49932887540240001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.58425392870920001</c:v>
+                  <c:v>0.48964135727449998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.53227042279350001</c:v>
+                  <c:v>0.37648172890909998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.48980424001869999</c:v>
+                  <c:v>0.32350813634699999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.73025348365450005</c:v>
+                  <c:v>0.27052430519550003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.7331210458563</c:v>
+                  <c:v>0.49518678690250001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.58420106096680002</c:v>
+                  <c:v>0.48483829699800002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.59116965124190002</c:v>
+                  <c:v>0.3686266592145</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.54492962852030002</c:v>
+                  <c:v>0.31507954093340002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.56385624898730002</c:v>
+                  <c:v>0.26111821018469999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1625,11 +1625,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103106816"/>
-        <c:axId val="103137664"/>
+        <c:axId val="43596032"/>
+        <c:axId val="43626880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103106816"/>
+        <c:axId val="43596032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1651,13 +1651,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103137664"/>
+        <c:crossAx val="43626880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1665,10 +1666,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103137664"/>
+        <c:axId val="43626880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1689,13 +1689,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103106816"/>
+        <c:crossAx val="43596032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7863,7 +7864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
@@ -7888,32 +7889,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="94" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="95"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="98" t="s">
+      <c r="E1" s="122"/>
+      <c r="F1" s="123" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="124"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="96"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="125"/>
       <c r="O1" s="63" t="s">
         <v>32</v>
       </c>
@@ -7940,17 +7941,17 @@
       <c r="AJ1" s="28"/>
       <c r="AK1" s="28"/>
       <c r="AL1" s="29"/>
-      <c r="AM1" s="91" t="s">
+      <c r="AM1" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" s="88" t="s">
+      <c r="AN1" s="117" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:40" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="89"/>
-      <c r="B2" s="97"/>
-      <c r="C2" s="90"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="119"/>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
@@ -8056,8 +8057,8 @@
       <c r="AL2" s="21">
         <v>24</v>
       </c>
-      <c r="AM2" s="91"/>
-      <c r="AN2" s="88"/>
+      <c r="AM2" s="120"/>
+      <c r="AN2" s="117"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -8102,99 +8103,99 @@
       <c r="N3" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="122">
+      <c r="O3" s="106">
         <f>$O$29/2</f>
         <v>2.633</v>
       </c>
-      <c r="P3" s="123">
+      <c r="P3" s="107">
         <f>$P$29/2</f>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q3" s="122">
+      <c r="Q3" s="106">
         <f>Q$29/2</f>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R3" s="123">
+      <c r="R3" s="107">
         <f>R$29/2</f>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S3" s="123">
+      <c r="S3" s="107">
         <f>S$29/2</f>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T3" s="122">
+      <c r="T3" s="106">
         <f>T$29/2</f>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U3" s="122">
+      <c r="U3" s="106">
         <f t="shared" ref="U3:AB18" si="1">U$29/2</f>
         <v>1.84</v>
       </c>
-      <c r="V3" s="122">
+      <c r="V3" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W3" s="124">
+      <c r="W3" s="108">
         <f>W$29/2</f>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X3" s="125">
+      <c r="X3" s="109">
         <f>X$29/2</f>
         <v>1.5445</v>
       </c>
-      <c r="Y3" s="126">
+      <c r="Y3" s="110">
         <f t="shared" ref="Y3:AE18" si="2">Y$29</f>
         <v>2.8820000000000001</v>
       </c>
-      <c r="Z3" s="125">
+      <c r="Z3" s="109">
         <f t="shared" si="2"/>
         <v>2.6960000000000002</v>
       </c>
-      <c r="AA3" s="125">
+      <c r="AA3" s="109">
         <f t="shared" si="2"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB3" s="125">
+      <c r="AB3" s="109">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC3" s="125">
+      <c r="AC3" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD3" s="125">
+      <c r="AD3" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE3" s="125">
+      <c r="AE3" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF3" s="122">
+      <c r="AF3" s="106">
         <f>AF$29</f>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG3" s="122">
+      <c r="AG3" s="106">
         <f t="shared" ref="AG3:AL18" si="3">AG$29</f>
         <v>0.91</v>
       </c>
-      <c r="AH3" s="122">
+      <c r="AH3" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI3" s="122">
+      <c r="AI3" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ3" s="122">
+      <c r="AJ3" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK3" s="122">
+      <c r="AK3" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL3" s="122">
+      <c r="AL3" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -8205,7 +8206,7 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18">
         <v>2</v>
@@ -8249,99 +8250,99 @@
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="122">
+      <c r="O4" s="106">
         <f t="shared" ref="O4:O23" si="5">$O$29/2</f>
         <v>2.633</v>
       </c>
-      <c r="P4" s="123">
+      <c r="P4" s="107">
         <f t="shared" ref="P4:P23" si="6">$P$29/2</f>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q4" s="122">
+      <c r="Q4" s="106">
         <f t="shared" ref="Q4:R19" si="7">Q$29/2</f>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R4" s="123">
+      <c r="R4" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S4" s="123">
+      <c r="S4" s="107">
         <f t="shared" ref="S4:X19" si="8">S$29/2</f>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T4" s="122">
+      <c r="T4" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U4" s="122">
+      <c r="U4" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V4" s="122">
+      <c r="V4" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W4" s="122">
+      <c r="W4" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X4" s="124">
+      <c r="X4" s="108">
         <f>X$29/2</f>
         <v>1.5445</v>
       </c>
-      <c r="Y4" s="125">
+      <c r="Y4" s="109">
         <f>Y$29/2</f>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z4" s="126">
+      <c r="Z4" s="110">
         <f t="shared" si="2"/>
         <v>2.6960000000000002</v>
       </c>
-      <c r="AA4" s="125">
+      <c r="AA4" s="109">
         <f t="shared" si="2"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB4" s="125">
+      <c r="AB4" s="109">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC4" s="125">
+      <c r="AC4" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD4" s="125">
+      <c r="AD4" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE4" s="125">
+      <c r="AE4" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF4" s="122">
+      <c r="AF4" s="106">
         <f t="shared" ref="AF4:AL23" si="9">AF$29</f>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG4" s="122">
+      <c r="AG4" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH4" s="122">
+      <c r="AH4" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI4" s="122">
+      <c r="AI4" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ4" s="122">
+      <c r="AJ4" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK4" s="122">
+      <c r="AK4" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL4" s="122">
+      <c r="AL4" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -8349,7 +8350,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="18">
         <v>3</v>
@@ -8393,99 +8394,99 @@
       <c r="N5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="122">
+      <c r="O5" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P5" s="123">
+      <c r="P5" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q5" s="122">
+      <c r="Q5" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R5" s="123">
+      <c r="R5" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S5" s="123">
+      <c r="S5" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T5" s="122">
+      <c r="T5" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U5" s="122">
+      <c r="U5" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V5" s="122">
+      <c r="V5" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W5" s="122">
+      <c r="W5" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X5" s="122">
+      <c r="X5" s="106">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y5" s="124">
+      <c r="Y5" s="108">
         <f>Y$29/2</f>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z5" s="125">
+      <c r="Z5" s="109">
         <f>Z$29/2</f>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA5" s="126">
+      <c r="AA5" s="110">
         <f t="shared" si="2"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB5" s="125">
+      <c r="AB5" s="109">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC5" s="125">
+      <c r="AC5" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD5" s="125">
+      <c r="AD5" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE5" s="125">
+      <c r="AE5" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF5" s="122">
+      <c r="AF5" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG5" s="122">
+      <c r="AG5" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH5" s="122">
+      <c r="AH5" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI5" s="122">
+      <c r="AI5" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ5" s="122">
+      <c r="AJ5" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK5" s="122">
+      <c r="AK5" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL5" s="122">
+      <c r="AL5" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -8534,99 +8535,99 @@
       <c r="N6" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="O6" s="122">
+      <c r="O6" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P6" s="123">
+      <c r="P6" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q6" s="122">
+      <c r="Q6" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R6" s="123">
+      <c r="R6" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S6" s="123">
+      <c r="S6" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T6" s="122">
+      <c r="T6" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U6" s="122">
+      <c r="U6" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V6" s="122">
+      <c r="V6" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W6" s="122">
+      <c r="W6" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X6" s="122">
+      <c r="X6" s="106">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y6" s="122">
+      <c r="Y6" s="106">
         <f t="shared" si="1"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z6" s="124">
+      <c r="Z6" s="108">
         <f>Z$29/2</f>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA6" s="125">
+      <c r="AA6" s="109">
         <f>AA$29/2</f>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB6" s="126">
+      <c r="AB6" s="110">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC6" s="125">
+      <c r="AC6" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD6" s="125">
+      <c r="AD6" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE6" s="125">
+      <c r="AE6" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF6" s="122">
+      <c r="AF6" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG6" s="122">
+      <c r="AG6" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH6" s="122">
+      <c r="AH6" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI6" s="122">
+      <c r="AI6" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ6" s="122">
+      <c r="AJ6" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK6" s="122">
+      <c r="AK6" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL6" s="122">
+      <c r="AL6" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -8634,7 +8635,7 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="18">
         <v>5</v>
@@ -8678,99 +8679,99 @@
       <c r="N7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O7" s="122">
+      <c r="O7" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P7" s="123">
+      <c r="P7" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q7" s="122">
+      <c r="Q7" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R7" s="123">
+      <c r="R7" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S7" s="123">
+      <c r="S7" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T7" s="122">
+      <c r="T7" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U7" s="122">
+      <c r="U7" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V7" s="122">
+      <c r="V7" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W7" s="122">
+      <c r="W7" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X7" s="122">
+      <c r="X7" s="106">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y7" s="122">
+      <c r="Y7" s="106">
         <f t="shared" si="1"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z7" s="122">
+      <c r="Z7" s="106">
         <f t="shared" si="1"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA7" s="124">
+      <c r="AA7" s="108">
         <f>AA$29/2</f>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB7" s="125">
+      <c r="AB7" s="109">
         <f>AB$29/2</f>
         <v>1.0385</v>
       </c>
-      <c r="AC7" s="126">
+      <c r="AC7" s="110">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD7" s="125">
+      <c r="AD7" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE7" s="125">
+      <c r="AE7" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF7" s="122">
+      <c r="AF7" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG7" s="122">
+      <c r="AG7" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH7" s="122">
+      <c r="AH7" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI7" s="122">
+      <c r="AI7" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ7" s="122">
+      <c r="AJ7" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK7" s="122">
+      <c r="AK7" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL7" s="122">
+      <c r="AL7" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -8778,7 +8779,7 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="18">
         <v>6</v>
@@ -8822,99 +8823,99 @@
       <c r="N8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O8" s="122">
+      <c r="O8" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P8" s="123">
+      <c r="P8" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q8" s="122">
+      <c r="Q8" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R8" s="123">
+      <c r="R8" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S8" s="123">
+      <c r="S8" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T8" s="122">
+      <c r="T8" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U8" s="122">
+      <c r="U8" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V8" s="122">
+      <c r="V8" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W8" s="122">
+      <c r="W8" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X8" s="122">
+      <c r="X8" s="106">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y8" s="122">
+      <c r="Y8" s="106">
         <f t="shared" si="1"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z8" s="122">
+      <c r="Z8" s="106">
         <f t="shared" si="1"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA8" s="122">
+      <c r="AA8" s="106">
         <f t="shared" si="1"/>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB8" s="124">
+      <c r="AB8" s="108">
         <f>AB$29/2</f>
         <v>1.0385</v>
       </c>
-      <c r="AC8" s="125">
+      <c r="AC8" s="109">
         <f>AC$29/2</f>
         <v>0.83599999999999997</v>
       </c>
-      <c r="AD8" s="126">
+      <c r="AD8" s="110">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE8" s="125">
+      <c r="AE8" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF8" s="122">
+      <c r="AF8" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG8" s="122">
+      <c r="AG8" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH8" s="122">
+      <c r="AH8" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI8" s="122">
+      <c r="AI8" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ8" s="122">
+      <c r="AJ8" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK8" s="122">
+      <c r="AK8" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL8" s="122">
+      <c r="AL8" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -8922,7 +8923,7 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="13">
         <v>7</v>
@@ -8966,99 +8967,99 @@
       <c r="N9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="O9" s="127">
+      <c r="O9" s="111">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P9" s="128">
+      <c r="P9" s="112">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q9" s="129">
+      <c r="Q9" s="113">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R9" s="128">
+      <c r="R9" s="112">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S9" s="128">
+      <c r="S9" s="112">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T9" s="129">
+      <c r="T9" s="113">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U9" s="129">
+      <c r="U9" s="113">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V9" s="129">
+      <c r="V9" s="113">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W9" s="129">
+      <c r="W9" s="113">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X9" s="129">
+      <c r="X9" s="113">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y9" s="129">
+      <c r="Y9" s="113">
         <f t="shared" si="1"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z9" s="129">
+      <c r="Z9" s="113">
         <f t="shared" si="1"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA9" s="129">
+      <c r="AA9" s="113">
         <f t="shared" si="1"/>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB9" s="129">
+      <c r="AB9" s="113">
         <f t="shared" si="1"/>
         <v>1.0385</v>
       </c>
-      <c r="AC9" s="130">
+      <c r="AC9" s="114">
         <f>AC$29/2</f>
         <v>0.83599999999999997</v>
       </c>
-      <c r="AD9" s="129">
+      <c r="AD9" s="113">
         <f>AD$29/2</f>
         <v>0.68</v>
       </c>
-      <c r="AE9" s="131">
+      <c r="AE9" s="115">
         <f>AE$29</f>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF9" s="129">
+      <c r="AF9" s="113">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG9" s="129">
+      <c r="AG9" s="113">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH9" s="129">
+      <c r="AH9" s="113">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI9" s="129">
+      <c r="AI9" s="113">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ9" s="129">
+      <c r="AJ9" s="113">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK9" s="129">
+      <c r="AK9" s="113">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL9" s="132">
+      <c r="AL9" s="116">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -9108,99 +9109,99 @@
         <v>0.39214855000000004</v>
       </c>
       <c r="N10" s="72"/>
-      <c r="O10" s="122">
+      <c r="O10" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P10" s="123">
+      <c r="P10" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q10" s="122">
+      <c r="Q10" s="106">
         <f>Q$29/2</f>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R10" s="123">
+      <c r="R10" s="107">
         <f>R$29/2</f>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S10" s="123">
+      <c r="S10" s="107">
         <f>S$29/2</f>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T10" s="122">
+      <c r="T10" s="106">
         <f>T$29/2</f>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U10" s="122">
+      <c r="U10" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V10" s="122">
+      <c r="V10" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W10" s="124">
+      <c r="W10" s="108">
         <f>W$29/2</f>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X10" s="125">
+      <c r="X10" s="109">
         <f>X$29/2</f>
         <v>1.5445</v>
       </c>
-      <c r="Y10" s="126">
+      <c r="Y10" s="110">
         <f t="shared" si="2"/>
         <v>2.8820000000000001</v>
       </c>
-      <c r="Z10" s="125">
+      <c r="Z10" s="109">
         <f t="shared" si="2"/>
         <v>2.6960000000000002</v>
       </c>
-      <c r="AA10" s="125">
+      <c r="AA10" s="109">
         <f t="shared" si="2"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB10" s="125">
+      <c r="AB10" s="109">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC10" s="125">
+      <c r="AC10" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD10" s="125">
+      <c r="AD10" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE10" s="125">
+      <c r="AE10" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF10" s="122">
+      <c r="AF10" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG10" s="122">
+      <c r="AG10" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH10" s="122">
+      <c r="AH10" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI10" s="122">
+      <c r="AI10" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ10" s="122">
+      <c r="AJ10" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK10" s="122">
+      <c r="AK10" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL10" s="122">
+      <c r="AL10" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -9211,7 +9212,7 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="18">
         <v>9</v>
@@ -9255,99 +9256,99 @@
       <c r="N11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O11" s="122">
+      <c r="O11" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P11" s="123">
+      <c r="P11" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q11" s="122">
+      <c r="Q11" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R11" s="123">
+      <c r="R11" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S11" s="123">
+      <c r="S11" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T11" s="122">
+      <c r="T11" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U11" s="122">
+      <c r="U11" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V11" s="122">
+      <c r="V11" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W11" s="122">
+      <c r="W11" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X11" s="124">
+      <c r="X11" s="108">
         <f>X$29/2</f>
         <v>1.5445</v>
       </c>
-      <c r="Y11" s="125">
+      <c r="Y11" s="109">
         <f>Y$29/2</f>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z11" s="126">
+      <c r="Z11" s="110">
         <f t="shared" si="2"/>
         <v>2.6960000000000002</v>
       </c>
-      <c r="AA11" s="125">
+      <c r="AA11" s="109">
         <f t="shared" si="2"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB11" s="125">
+      <c r="AB11" s="109">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC11" s="125">
+      <c r="AC11" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD11" s="125">
+      <c r="AD11" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE11" s="125">
+      <c r="AE11" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF11" s="122">
+      <c r="AF11" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG11" s="122">
+      <c r="AG11" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH11" s="122">
+      <c r="AH11" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI11" s="122">
+      <c r="AI11" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ11" s="122">
+      <c r="AJ11" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK11" s="122">
+      <c r="AK11" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL11" s="122">
+      <c r="AL11" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -9355,7 +9356,7 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="18">
         <v>10</v>
@@ -9399,99 +9400,99 @@
       <c r="N12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O12" s="122">
+      <c r="O12" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P12" s="123">
+      <c r="P12" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q12" s="122">
+      <c r="Q12" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R12" s="123">
+      <c r="R12" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S12" s="123">
+      <c r="S12" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T12" s="122">
+      <c r="T12" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U12" s="122">
+      <c r="U12" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V12" s="122">
+      <c r="V12" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W12" s="122">
+      <c r="W12" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X12" s="122">
+      <c r="X12" s="106">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y12" s="124">
+      <c r="Y12" s="108">
         <f>Y$29/2</f>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z12" s="125">
+      <c r="Z12" s="109">
         <f>Z$29/2</f>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA12" s="126">
+      <c r="AA12" s="110">
         <f t="shared" si="2"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB12" s="125">
+      <c r="AB12" s="109">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC12" s="125">
+      <c r="AC12" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD12" s="125">
+      <c r="AD12" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE12" s="125">
+      <c r="AE12" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF12" s="122">
+      <c r="AF12" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG12" s="122">
+      <c r="AG12" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH12" s="122">
+      <c r="AH12" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI12" s="122">
+      <c r="AI12" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ12" s="122">
+      <c r="AJ12" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK12" s="122">
+      <c r="AK12" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL12" s="122">
+      <c r="AL12" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -9538,99 +9539,99 @@
         <v>0.14001290000000002</v>
       </c>
       <c r="N13" s="72"/>
-      <c r="O13" s="122">
+      <c r="O13" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P13" s="123">
+      <c r="P13" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q13" s="122">
+      <c r="Q13" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R13" s="123">
+      <c r="R13" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S13" s="123">
+      <c r="S13" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T13" s="122">
+      <c r="T13" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U13" s="122">
+      <c r="U13" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V13" s="122">
+      <c r="V13" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W13" s="122">
+      <c r="W13" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X13" s="122">
+      <c r="X13" s="106">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y13" s="122">
+      <c r="Y13" s="106">
         <f t="shared" si="1"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z13" s="124">
+      <c r="Z13" s="108">
         <f>Z$29/2</f>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA13" s="125">
+      <c r="AA13" s="109">
         <f>AA$29/2</f>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB13" s="126">
+      <c r="AB13" s="110">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC13" s="125">
+      <c r="AC13" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD13" s="125">
+      <c r="AD13" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE13" s="125">
+      <c r="AE13" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF13" s="122">
+      <c r="AF13" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG13" s="122">
+      <c r="AG13" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH13" s="122">
+      <c r="AH13" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI13" s="122">
+      <c r="AI13" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ13" s="122">
+      <c r="AJ13" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK13" s="122">
+      <c r="AK13" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL13" s="122">
+      <c r="AL13" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -9638,7 +9639,7 @@
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="18">
         <v>12</v>
@@ -9682,99 +9683,99 @@
       <c r="N14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O14" s="122">
+      <c r="O14" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P14" s="123">
+      <c r="P14" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q14" s="122">
+      <c r="Q14" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R14" s="123">
+      <c r="R14" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S14" s="123">
+      <c r="S14" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T14" s="122">
+      <c r="T14" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U14" s="122">
+      <c r="U14" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V14" s="122">
+      <c r="V14" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W14" s="122">
+      <c r="W14" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X14" s="122">
+      <c r="X14" s="106">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y14" s="122">
+      <c r="Y14" s="106">
         <f t="shared" si="1"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z14" s="122">
+      <c r="Z14" s="106">
         <f t="shared" si="1"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA14" s="124">
+      <c r="AA14" s="108">
         <f>AA$29/2</f>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB14" s="125">
+      <c r="AB14" s="109">
         <f>AB$29/2</f>
         <v>1.0385</v>
       </c>
-      <c r="AC14" s="126">
+      <c r="AC14" s="110">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD14" s="125">
+      <c r="AD14" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE14" s="125">
+      <c r="AE14" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF14" s="122">
+      <c r="AF14" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG14" s="122">
+      <c r="AG14" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH14" s="122">
+      <c r="AH14" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI14" s="122">
+      <c r="AI14" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ14" s="122">
+      <c r="AJ14" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK14" s="122">
+      <c r="AK14" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL14" s="122">
+      <c r="AL14" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -9782,7 +9783,7 @@
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="18">
         <v>13</v>
@@ -9826,99 +9827,99 @@
       <c r="N15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O15" s="122">
+      <c r="O15" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P15" s="123">
+      <c r="P15" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q15" s="122">
+      <c r="Q15" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R15" s="123">
+      <c r="R15" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S15" s="123">
+      <c r="S15" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T15" s="122">
+      <c r="T15" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U15" s="122">
+      <c r="U15" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V15" s="122">
+      <c r="V15" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W15" s="122">
+      <c r="W15" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X15" s="122">
+      <c r="X15" s="106">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y15" s="122">
+      <c r="Y15" s="106">
         <f t="shared" si="1"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z15" s="122">
+      <c r="Z15" s="106">
         <f t="shared" si="1"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA15" s="122">
+      <c r="AA15" s="106">
         <f t="shared" si="1"/>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB15" s="124">
+      <c r="AB15" s="108">
         <f>AB$29/2</f>
         <v>1.0385</v>
       </c>
-      <c r="AC15" s="125">
+      <c r="AC15" s="109">
         <f>AC$29/2</f>
         <v>0.83599999999999997</v>
       </c>
-      <c r="AD15" s="126">
+      <c r="AD15" s="110">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE15" s="125">
+      <c r="AE15" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF15" s="122">
+      <c r="AF15" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG15" s="122">
+      <c r="AG15" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH15" s="122">
+      <c r="AH15" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI15" s="122">
+      <c r="AI15" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ15" s="122">
+      <c r="AJ15" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK15" s="122">
+      <c r="AK15" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL15" s="122">
+      <c r="AL15" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -9926,7 +9927,7 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="13">
         <v>14</v>
@@ -9970,99 +9971,99 @@
       <c r="N16" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="O16" s="127">
+      <c r="O16" s="111">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P16" s="128">
+      <c r="P16" s="112">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q16" s="129">
+      <c r="Q16" s="113">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R16" s="128">
+      <c r="R16" s="112">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S16" s="128">
+      <c r="S16" s="112">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T16" s="129">
+      <c r="T16" s="113">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U16" s="129">
+      <c r="U16" s="113">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V16" s="129">
+      <c r="V16" s="113">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W16" s="129">
+      <c r="W16" s="113">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X16" s="129">
+      <c r="X16" s="113">
         <f t="shared" si="1"/>
         <v>1.5445</v>
       </c>
-      <c r="Y16" s="129">
+      <c r="Y16" s="113">
         <f t="shared" si="1"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z16" s="129">
+      <c r="Z16" s="113">
         <f t="shared" si="1"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA16" s="129">
+      <c r="AA16" s="113">
         <f t="shared" si="1"/>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB16" s="129">
+      <c r="AB16" s="113">
         <f t="shared" si="1"/>
         <v>1.0385</v>
       </c>
-      <c r="AC16" s="130">
+      <c r="AC16" s="114">
         <f>AC$29/2</f>
         <v>0.83599999999999997</v>
       </c>
-      <c r="AD16" s="129">
+      <c r="AD16" s="113">
         <f>AD$29/2</f>
         <v>0.68</v>
       </c>
-      <c r="AE16" s="131">
+      <c r="AE16" s="115">
         <f>AE$29</f>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF16" s="129">
+      <c r="AF16" s="113">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG16" s="129">
+      <c r="AG16" s="113">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH16" s="129">
+      <c r="AH16" s="113">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI16" s="129">
+      <c r="AI16" s="113">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ16" s="129">
+      <c r="AJ16" s="113">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK16" s="129">
+      <c r="AK16" s="113">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL16" s="132">
+      <c r="AL16" s="116">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -10109,99 +10110,99 @@
         <v>0.44311704999999996</v>
       </c>
       <c r="N17" s="72"/>
-      <c r="O17" s="122">
+      <c r="O17" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P17" s="123">
+      <c r="P17" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q17" s="122">
+      <c r="Q17" s="106">
         <f>Q$29/2</f>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R17" s="123">
+      <c r="R17" s="107">
         <f>R$29/2</f>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S17" s="123">
+      <c r="S17" s="107">
         <f>S$29/2</f>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T17" s="122">
+      <c r="T17" s="106">
         <f>T$29/2</f>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U17" s="122">
+      <c r="U17" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V17" s="122">
+      <c r="V17" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W17" s="124">
+      <c r="W17" s="108">
         <f>W$29/2</f>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X17" s="125">
+      <c r="X17" s="109">
         <f>X$29/2</f>
         <v>1.5445</v>
       </c>
-      <c r="Y17" s="126">
+      <c r="Y17" s="110">
         <f t="shared" si="2"/>
         <v>2.8820000000000001</v>
       </c>
-      <c r="Z17" s="125">
+      <c r="Z17" s="109">
         <f t="shared" si="2"/>
         <v>2.6960000000000002</v>
       </c>
-      <c r="AA17" s="125">
+      <c r="AA17" s="109">
         <f t="shared" si="2"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB17" s="125">
+      <c r="AB17" s="109">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC17" s="125">
+      <c r="AC17" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD17" s="125">
+      <c r="AD17" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE17" s="125">
+      <c r="AE17" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF17" s="122">
+      <c r="AF17" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG17" s="122">
+      <c r="AG17" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH17" s="122">
+      <c r="AH17" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI17" s="122">
+      <c r="AI17" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ17" s="122">
+      <c r="AJ17" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK17" s="122">
+      <c r="AK17" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL17" s="122">
+      <c r="AL17" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -10211,7 +10212,7 @@
       <c r="AN17" s="41"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="104" t="s">
+      <c r="A18" s="88" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="18">
@@ -10256,99 +10257,99 @@
       <c r="N18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O18" s="122">
+      <c r="O18" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P18" s="123">
+      <c r="P18" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q18" s="122">
+      <c r="Q18" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R18" s="123">
+      <c r="R18" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S18" s="123">
+      <c r="S18" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T18" s="122">
+      <c r="T18" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U18" s="122">
+      <c r="U18" s="106">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="V18" s="122">
+      <c r="V18" s="106">
         <f t="shared" si="1"/>
         <v>1.74</v>
       </c>
-      <c r="W18" s="122">
+      <c r="W18" s="106">
         <f t="shared" si="1"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X18" s="124">
+      <c r="X18" s="108">
         <f>X$29/2</f>
         <v>1.5445</v>
       </c>
-      <c r="Y18" s="125">
+      <c r="Y18" s="109">
         <f>Y$29/2</f>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z18" s="126">
+      <c r="Z18" s="110">
         <f t="shared" si="2"/>
         <v>2.6960000000000002</v>
       </c>
-      <c r="AA18" s="125">
+      <c r="AA18" s="109">
         <f t="shared" si="2"/>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB18" s="125">
+      <c r="AB18" s="109">
         <f t="shared" si="2"/>
         <v>2.077</v>
       </c>
-      <c r="AC18" s="125">
+      <c r="AC18" s="109">
         <f t="shared" si="2"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD18" s="125">
+      <c r="AD18" s="109">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="AE18" s="125">
+      <c r="AE18" s="109">
         <f t="shared" si="2"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF18" s="122">
+      <c r="AF18" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG18" s="122">
+      <c r="AG18" s="106">
         <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
-      <c r="AH18" s="122">
+      <c r="AH18" s="106">
         <f t="shared" si="3"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI18" s="122">
+      <c r="AI18" s="106">
         <f t="shared" si="3"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ18" s="122">
+      <c r="AJ18" s="106">
         <f t="shared" si="3"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK18" s="122">
+      <c r="AK18" s="106">
         <f t="shared" si="3"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL18" s="122">
+      <c r="AL18" s="106">
         <f t="shared" si="3"/>
         <v>0.50800000000000001</v>
       </c>
@@ -10400,99 +10401,99 @@
       <c r="N19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O19" s="122">
+      <c r="O19" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P19" s="123">
+      <c r="P19" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q19" s="122">
+      <c r="Q19" s="106">
         <f t="shared" si="7"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R19" s="123">
+      <c r="R19" s="107">
         <f t="shared" si="7"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S19" s="123">
+      <c r="S19" s="107">
         <f t="shared" si="8"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T19" s="122">
+      <c r="T19" s="106">
         <f t="shared" si="8"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U19" s="122">
+      <c r="U19" s="106">
         <f t="shared" si="8"/>
         <v>1.84</v>
       </c>
-      <c r="V19" s="122">
+      <c r="V19" s="106">
         <f t="shared" si="8"/>
         <v>1.74</v>
       </c>
-      <c r="W19" s="122">
+      <c r="W19" s="106">
         <f t="shared" si="8"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X19" s="122">
+      <c r="X19" s="106">
         <f t="shared" si="8"/>
         <v>1.5445</v>
       </c>
-      <c r="Y19" s="124">
+      <c r="Y19" s="108">
         <f>Y$29/2</f>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z19" s="125">
+      <c r="Z19" s="109">
         <f>Z$29/2</f>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA19" s="126">
+      <c r="AA19" s="110">
         <f t="shared" ref="AA19:AE22" si="10">AA$29</f>
         <v>2.4980000000000002</v>
       </c>
-      <c r="AB19" s="125">
+      <c r="AB19" s="109">
         <f t="shared" si="10"/>
         <v>2.077</v>
       </c>
-      <c r="AC19" s="125">
+      <c r="AC19" s="109">
         <f t="shared" si="10"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD19" s="125">
+      <c r="AD19" s="109">
         <f t="shared" si="10"/>
         <v>1.36</v>
       </c>
-      <c r="AE19" s="125">
+      <c r="AE19" s="109">
         <f t="shared" si="10"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF19" s="122">
+      <c r="AF19" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG19" s="122">
+      <c r="AG19" s="106">
         <f t="shared" si="9"/>
         <v>0.91</v>
       </c>
-      <c r="AH19" s="122">
+      <c r="AH19" s="106">
         <f t="shared" si="9"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI19" s="122">
+      <c r="AI19" s="106">
         <f t="shared" si="9"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ19" s="122">
+      <c r="AJ19" s="106">
         <f t="shared" si="9"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK19" s="122">
+      <c r="AK19" s="106">
         <f t="shared" si="9"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL19" s="122">
+      <c r="AL19" s="106">
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
@@ -10539,99 +10540,99 @@
         <v>9.7921600000000011E-2</v>
       </c>
       <c r="N20" s="72"/>
-      <c r="O20" s="122">
+      <c r="O20" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P20" s="123">
+      <c r="P20" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q20" s="122">
+      <c r="Q20" s="106">
         <f t="shared" ref="Q20:AB23" si="11">Q$29/2</f>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R20" s="123">
+      <c r="R20" s="107">
         <f t="shared" si="11"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S20" s="123">
+      <c r="S20" s="107">
         <f t="shared" si="11"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T20" s="122">
+      <c r="T20" s="106">
         <f t="shared" si="11"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U20" s="122">
+      <c r="U20" s="106">
         <f t="shared" si="11"/>
         <v>1.84</v>
       </c>
-      <c r="V20" s="122">
+      <c r="V20" s="106">
         <f t="shared" si="11"/>
         <v>1.74</v>
       </c>
-      <c r="W20" s="122">
+      <c r="W20" s="106">
         <f t="shared" si="11"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X20" s="122">
+      <c r="X20" s="106">
         <f t="shared" si="11"/>
         <v>1.5445</v>
       </c>
-      <c r="Y20" s="122">
+      <c r="Y20" s="106">
         <f t="shared" si="11"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z20" s="124">
+      <c r="Z20" s="108">
         <f>Z$29/2</f>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA20" s="125">
+      <c r="AA20" s="109">
         <f>AA$29/2</f>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB20" s="126">
+      <c r="AB20" s="110">
         <f t="shared" si="10"/>
         <v>2.077</v>
       </c>
-      <c r="AC20" s="125">
+      <c r="AC20" s="109">
         <f t="shared" si="10"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD20" s="125">
+      <c r="AD20" s="109">
         <f t="shared" si="10"/>
         <v>1.36</v>
       </c>
-      <c r="AE20" s="125">
+      <c r="AE20" s="109">
         <f t="shared" si="10"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF20" s="122">
+      <c r="AF20" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG20" s="122">
+      <c r="AG20" s="106">
         <f t="shared" si="9"/>
         <v>0.91</v>
       </c>
-      <c r="AH20" s="122">
+      <c r="AH20" s="106">
         <f t="shared" si="9"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI20" s="122">
+      <c r="AI20" s="106">
         <f t="shared" si="9"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ20" s="122">
+      <c r="AJ20" s="106">
         <f t="shared" si="9"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK20" s="122">
+      <c r="AK20" s="106">
         <f t="shared" si="9"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL20" s="122">
+      <c r="AL20" s="106">
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
@@ -10683,99 +10684,99 @@
       <c r="N21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O21" s="122">
+      <c r="O21" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P21" s="123">
+      <c r="P21" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q21" s="122">
+      <c r="Q21" s="106">
         <f t="shared" si="11"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R21" s="123">
+      <c r="R21" s="107">
         <f t="shared" si="11"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S21" s="123">
+      <c r="S21" s="107">
         <f t="shared" si="11"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T21" s="122">
+      <c r="T21" s="106">
         <f t="shared" si="11"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U21" s="122">
+      <c r="U21" s="106">
         <f t="shared" si="11"/>
         <v>1.84</v>
       </c>
-      <c r="V21" s="122">
+      <c r="V21" s="106">
         <f t="shared" si="11"/>
         <v>1.74</v>
       </c>
-      <c r="W21" s="122">
+      <c r="W21" s="106">
         <f t="shared" si="11"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X21" s="122">
+      <c r="X21" s="106">
         <f t="shared" si="11"/>
         <v>1.5445</v>
       </c>
-      <c r="Y21" s="122">
+      <c r="Y21" s="106">
         <f t="shared" si="11"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z21" s="122">
+      <c r="Z21" s="106">
         <f t="shared" si="11"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA21" s="124">
+      <c r="AA21" s="108">
         <f>AA$29/2</f>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB21" s="125">
+      <c r="AB21" s="109">
         <f>AB$29/2</f>
         <v>1.0385</v>
       </c>
-      <c r="AC21" s="126">
+      <c r="AC21" s="110">
         <f t="shared" si="10"/>
         <v>1.6719999999999999</v>
       </c>
-      <c r="AD21" s="125">
+      <c r="AD21" s="109">
         <f t="shared" si="10"/>
         <v>1.36</v>
       </c>
-      <c r="AE21" s="125">
+      <c r="AE21" s="109">
         <f t="shared" si="10"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF21" s="122">
+      <c r="AF21" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG21" s="122">
+      <c r="AG21" s="106">
         <f t="shared" si="9"/>
         <v>0.91</v>
       </c>
-      <c r="AH21" s="122">
+      <c r="AH21" s="106">
         <f t="shared" si="9"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI21" s="122">
+      <c r="AI21" s="106">
         <f t="shared" si="9"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ21" s="122">
+      <c r="AJ21" s="106">
         <f t="shared" si="9"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK21" s="122">
+      <c r="AK21" s="106">
         <f t="shared" si="9"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL21" s="122">
+      <c r="AL21" s="106">
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
@@ -10827,99 +10828,99 @@
       <c r="N22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O22" s="122">
+      <c r="O22" s="106">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P22" s="123">
+      <c r="P22" s="107">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q22" s="122">
+      <c r="Q22" s="106">
         <f t="shared" si="11"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R22" s="123">
+      <c r="R22" s="107">
         <f t="shared" si="11"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S22" s="123">
+      <c r="S22" s="107">
         <f t="shared" si="11"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T22" s="122">
+      <c r="T22" s="106">
         <f t="shared" si="11"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U22" s="122">
+      <c r="U22" s="106">
         <f t="shared" si="11"/>
         <v>1.84</v>
       </c>
-      <c r="V22" s="122">
+      <c r="V22" s="106">
         <f t="shared" si="11"/>
         <v>1.74</v>
       </c>
-      <c r="W22" s="122">
+      <c r="W22" s="106">
         <f t="shared" si="11"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X22" s="122">
+      <c r="X22" s="106">
         <f t="shared" si="11"/>
         <v>1.5445</v>
       </c>
-      <c r="Y22" s="122">
+      <c r="Y22" s="106">
         <f t="shared" si="11"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z22" s="122">
+      <c r="Z22" s="106">
         <f t="shared" si="11"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA22" s="122">
+      <c r="AA22" s="106">
         <f t="shared" si="11"/>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB22" s="124">
+      <c r="AB22" s="108">
         <f>AB$29/2</f>
         <v>1.0385</v>
       </c>
-      <c r="AC22" s="125">
+      <c r="AC22" s="109">
         <f>AC$29/2</f>
         <v>0.83599999999999997</v>
       </c>
-      <c r="AD22" s="126">
+      <c r="AD22" s="110">
         <f t="shared" si="10"/>
         <v>1.36</v>
       </c>
-      <c r="AE22" s="125">
+      <c r="AE22" s="109">
         <f t="shared" si="10"/>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF22" s="122">
+      <c r="AF22" s="106">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG22" s="122">
+      <c r="AG22" s="106">
         <f t="shared" si="9"/>
         <v>0.91</v>
       </c>
-      <c r="AH22" s="122">
+      <c r="AH22" s="106">
         <f t="shared" si="9"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI22" s="122">
+      <c r="AI22" s="106">
         <f t="shared" si="9"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ22" s="122">
+      <c r="AJ22" s="106">
         <f t="shared" si="9"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK22" s="122">
+      <c r="AK22" s="106">
         <f t="shared" si="9"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL22" s="122">
+      <c r="AL22" s="106">
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
@@ -10971,185 +10972,185 @@
       <c r="N23" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="O23" s="127">
+      <c r="O23" s="111">
         <f t="shared" si="5"/>
         <v>2.633</v>
       </c>
-      <c r="P23" s="128">
+      <c r="P23" s="112">
         <f t="shared" si="6"/>
         <v>2.6324999999999998</v>
       </c>
-      <c r="Q23" s="129">
+      <c r="Q23" s="113">
         <f t="shared" si="11"/>
         <v>2.5045000000000002</v>
       </c>
-      <c r="R23" s="128">
+      <c r="R23" s="112">
         <f t="shared" si="11"/>
         <v>2.3704999999999998</v>
       </c>
-      <c r="S23" s="128">
+      <c r="S23" s="112">
         <f t="shared" si="11"/>
         <v>2.2124999999999999</v>
       </c>
-      <c r="T23" s="129">
+      <c r="T23" s="113">
         <f t="shared" si="11"/>
         <v>2.0455000000000001</v>
       </c>
-      <c r="U23" s="129">
+      <c r="U23" s="113">
         <f t="shared" si="11"/>
         <v>1.84</v>
       </c>
-      <c r="V23" s="129">
+      <c r="V23" s="113">
         <f t="shared" si="11"/>
         <v>1.74</v>
       </c>
-      <c r="W23" s="129">
+      <c r="W23" s="113">
         <f t="shared" si="11"/>
         <v>1.6425000000000001</v>
       </c>
-      <c r="X23" s="129">
+      <c r="X23" s="113">
         <f t="shared" si="11"/>
         <v>1.5445</v>
       </c>
-      <c r="Y23" s="129">
+      <c r="Y23" s="113">
         <f t="shared" si="11"/>
         <v>1.4410000000000001</v>
       </c>
-      <c r="Z23" s="129">
+      <c r="Z23" s="113">
         <f t="shared" si="11"/>
         <v>1.3480000000000001</v>
       </c>
-      <c r="AA23" s="129">
+      <c r="AA23" s="113">
         <f t="shared" si="11"/>
         <v>1.2490000000000001</v>
       </c>
-      <c r="AB23" s="129">
+      <c r="AB23" s="113">
         <f t="shared" si="11"/>
         <v>1.0385</v>
       </c>
-      <c r="AC23" s="130">
+      <c r="AC23" s="114">
         <f>AC$29/2</f>
         <v>0.83599999999999997</v>
       </c>
-      <c r="AD23" s="129">
+      <c r="AD23" s="113">
         <f>AD$29/2</f>
         <v>0.68</v>
       </c>
-      <c r="AE23" s="131">
+      <c r="AE23" s="115">
         <f>AE$29</f>
         <v>1.1379999999999999</v>
       </c>
-      <c r="AF23" s="129">
+      <c r="AF23" s="113">
         <f t="shared" si="9"/>
         <v>0.95399999999999996</v>
       </c>
-      <c r="AG23" s="129">
+      <c r="AG23" s="113">
         <f t="shared" si="9"/>
         <v>0.91</v>
       </c>
-      <c r="AH23" s="129">
+      <c r="AH23" s="113">
         <f t="shared" si="9"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="AI23" s="129">
+      <c r="AI23" s="113">
         <f t="shared" si="9"/>
         <v>0.79600000000000004</v>
       </c>
-      <c r="AJ23" s="129">
+      <c r="AJ23" s="113">
         <f t="shared" si="9"/>
         <v>0.70699999999999996</v>
       </c>
-      <c r="AK23" s="129">
+      <c r="AK23" s="113">
         <f t="shared" si="9"/>
         <v>0.65100000000000002</v>
       </c>
-      <c r="AL23" s="132">
+      <c r="AL23" s="116">
         <f t="shared" si="9"/>
         <v>0.50800000000000001</v>
       </c>
       <c r="AN23" s="42"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="105" t="s">
+      <c r="A24" s="89" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="89">
+        <v>22</v>
+      </c>
+      <c r="C24" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="105">
-        <v>22</v>
-      </c>
-      <c r="C24" s="106" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="121">
+      <c r="D24" s="105">
         <v>10</v>
       </c>
-      <c r="E24" s="107">
+      <c r="E24" s="91">
         <v>12</v>
       </c>
-      <c r="F24" s="108">
+      <c r="F24" s="92">
         <v>0.245</v>
       </c>
-      <c r="G24" s="109">
+      <c r="G24" s="93">
         <v>0.24</v>
       </c>
-      <c r="H24" s="110">
+      <c r="H24" s="94">
         <v>1.25</v>
       </c>
-      <c r="I24" s="112">
+      <c r="I24" s="96">
         <v>11</v>
       </c>
-      <c r="J24" s="113">
+      <c r="J24" s="97">
         <v>0.5</v>
       </c>
-      <c r="K24" s="114">
+      <c r="K24" s="98">
         <f>K4</f>
         <v>2.8820000000000001</v>
       </c>
-      <c r="L24" s="114">
+      <c r="L24" s="98">
         <v>0</v>
       </c>
-      <c r="M24" s="114">
+      <c r="M24" s="98">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N24" s="106" t="s">
+      <c r="N24" s="90" t="s">
         <v>59</v>
       </c>
       <c r="O24" s="25"/>
       <c r="P24" s="30"/>
-      <c r="Q24" s="116"/>
-      <c r="R24" s="117"/>
-      <c r="S24" s="117"/>
-      <c r="T24" s="116"/>
-      <c r="U24" s="116"/>
-      <c r="V24" s="116"/>
-      <c r="W24" s="116"/>
-      <c r="X24" s="116"/>
-      <c r="Y24" s="116"/>
-      <c r="Z24" s="116"/>
-      <c r="AA24" s="116"/>
-      <c r="AB24" s="116"/>
-      <c r="AC24" s="117"/>
-      <c r="AD24" s="117"/>
-      <c r="AE24" s="117"/>
-      <c r="AF24" s="116"/>
-      <c r="AG24" s="116"/>
-      <c r="AH24" s="116"/>
-      <c r="AI24" s="116"/>
-      <c r="AJ24" s="116"/>
-      <c r="AK24" s="116"/>
-      <c r="AL24" s="118"/>
+      <c r="Q24" s="100"/>
+      <c r="R24" s="101"/>
+      <c r="S24" s="101"/>
+      <c r="T24" s="100"/>
+      <c r="U24" s="100"/>
+      <c r="V24" s="100"/>
+      <c r="W24" s="100"/>
+      <c r="X24" s="100"/>
+      <c r="Y24" s="100"/>
+      <c r="Z24" s="100"/>
+      <c r="AA24" s="100"/>
+      <c r="AB24" s="100"/>
+      <c r="AC24" s="101"/>
+      <c r="AD24" s="101"/>
+      <c r="AE24" s="101"/>
+      <c r="AF24" s="100"/>
+      <c r="AG24" s="100"/>
+      <c r="AH24" s="100"/>
+      <c r="AI24" s="100"/>
+      <c r="AJ24" s="100"/>
+      <c r="AK24" s="100"/>
+      <c r="AL24" s="102"/>
       <c r="AM24" s="20"/>
       <c r="AN24" s="41"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="18">
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1">
         <v>11</v>
@@ -11157,7 +11158,7 @@
       <c r="E25" s="3">
         <v>13</v>
       </c>
-      <c r="F25" s="111">
+      <c r="F25" s="95">
         <v>0.27400000000000002</v>
       </c>
       <c r="G25" s="60">
@@ -11166,7 +11167,7 @@
       <c r="H25" s="9">
         <v>1.25</v>
       </c>
-      <c r="I25" s="115">
+      <c r="I25" s="99">
         <v>12</v>
       </c>
       <c r="J25" s="79">
@@ -11189,8 +11190,8 @@
       <c r="O25" s="25"/>
       <c r="P25" s="30"/>
       <c r="Q25" s="27"/>
-      <c r="R25" s="119"/>
-      <c r="S25" s="119"/>
+      <c r="R25" s="103"/>
+      <c r="S25" s="103"/>
       <c r="T25" s="27"/>
       <c r="U25" s="27"/>
       <c r="V25" s="27"/>
@@ -11200,9 +11201,9 @@
       <c r="Z25" s="27"/>
       <c r="AA25" s="27"/>
       <c r="AB25" s="27"/>
-      <c r="AC25" s="119"/>
-      <c r="AD25" s="119"/>
-      <c r="AE25" s="119"/>
+      <c r="AC25" s="103"/>
+      <c r="AD25" s="103"/>
+      <c r="AE25" s="103"/>
       <c r="AF25" s="27"/>
       <c r="AG25" s="27"/>
       <c r="AH25" s="27"/>
@@ -11214,13 +11215,13 @@
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="18">
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1">
         <v>13</v>
@@ -11228,7 +11229,7 @@
       <c r="E26" s="3">
         <v>15</v>
       </c>
-      <c r="F26" s="111">
+      <c r="F26" s="95">
         <v>0.45200000000000001</v>
       </c>
       <c r="G26" s="60">
@@ -11237,7 +11238,7 @@
       <c r="H26" s="9">
         <v>1.25</v>
       </c>
-      <c r="I26" s="115">
+      <c r="I26" s="99">
         <v>14</v>
       </c>
       <c r="J26" s="79">
@@ -11260,8 +11261,8 @@
       <c r="O26" s="25"/>
       <c r="P26" s="30"/>
       <c r="Q26" s="27"/>
-      <c r="R26" s="119"/>
-      <c r="S26" s="119"/>
+      <c r="R26" s="103"/>
+      <c r="S26" s="103"/>
       <c r="T26" s="27"/>
       <c r="U26" s="27"/>
       <c r="V26" s="27"/>
@@ -11271,27 +11272,27 @@
       <c r="Z26" s="27"/>
       <c r="AA26" s="27"/>
       <c r="AB26" s="27"/>
-      <c r="AC26" s="119"/>
-      <c r="AD26" s="119"/>
-      <c r="AE26" s="119"/>
+      <c r="AC26" s="103"/>
+      <c r="AD26" s="103"/>
+      <c r="AE26" s="103"/>
       <c r="AF26" s="27"/>
       <c r="AG26" s="27"/>
       <c r="AH26" s="27"/>
       <c r="AI26" s="27"/>
       <c r="AJ26" s="27"/>
       <c r="AK26" s="27"/>
-      <c r="AL26" s="120"/>
+      <c r="AL26" s="104"/>
       <c r="AN26" s="41"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="18">
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1">
         <v>14</v>
@@ -11299,7 +11300,7 @@
       <c r="E27" s="3">
         <v>16</v>
       </c>
-      <c r="F27" s="111">
+      <c r="F27" s="95">
         <v>0.54</v>
       </c>
       <c r="G27" s="60">
@@ -11308,7 +11309,7 @@
       <c r="H27" s="9">
         <v>1.25</v>
       </c>
-      <c r="I27" s="115">
+      <c r="I27" s="99">
         <v>15</v>
       </c>
       <c r="J27" s="79">
@@ -11331,8 +11332,8 @@
       <c r="O27" s="25"/>
       <c r="P27" s="30"/>
       <c r="Q27" s="27"/>
-      <c r="R27" s="119"/>
-      <c r="S27" s="119"/>
+      <c r="R27" s="103"/>
+      <c r="S27" s="103"/>
       <c r="T27" s="27"/>
       <c r="U27" s="27"/>
       <c r="V27" s="27"/>
@@ -11342,27 +11343,27 @@
       <c r="Z27" s="27"/>
       <c r="AA27" s="27"/>
       <c r="AB27" s="27"/>
-      <c r="AC27" s="119"/>
-      <c r="AD27" s="119"/>
-      <c r="AE27" s="119"/>
+      <c r="AC27" s="103"/>
+      <c r="AD27" s="103"/>
+      <c r="AE27" s="103"/>
       <c r="AF27" s="27"/>
       <c r="AG27" s="27"/>
       <c r="AH27" s="27"/>
       <c r="AI27" s="27"/>
       <c r="AJ27" s="27"/>
       <c r="AK27" s="27"/>
-      <c r="AL27" s="120"/>
+      <c r="AL27" s="104"/>
       <c r="AN27" s="41"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="13">
         <v>26</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1">
         <v>15</v>
@@ -11427,7 +11428,7 @@
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="36">
         <v>0</v>
@@ -11815,7 +11816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11838,227 +11841,227 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="24">
-        <v>0.245</v>
-      </c>
-      <c r="C2" s="84">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D2" s="85">
-        <v>0.69280723872630001</v>
+        <v>0.56385624898730002</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B3" s="24">
-        <v>0.27400000000000002</v>
+        <v>0.245</v>
       </c>
       <c r="C3" s="84">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D3" s="85">
-        <v>0.68802083102529998</v>
+        <v>0.50484503415899995</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" s="24">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C4" s="84">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D4" s="85">
-        <v>0.55790288509749997</v>
+        <v>0.49601387384309997</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="24">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C5" s="84">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D5" s="85">
-        <v>0.50663002823820003</v>
+        <v>0.39042208149230001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="87">
-        <v>7</v>
+      <c r="A6" s="1">
+        <v>13</v>
       </c>
       <c r="B6" s="24">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C6" s="84">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D6" s="85">
-        <v>0.4682401240911</v>
+        <v>0.33874927541130001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>9</v>
+      <c r="A7" s="87">
+        <v>14</v>
       </c>
       <c r="B7" s="24">
-        <v>0.245</v>
+        <v>0.629</v>
       </c>
       <c r="C7" s="84">
         <v>0.75</v>
       </c>
       <c r="D7" s="85">
-        <v>0.70697489391379997</v>
+        <v>0.28565397168509998</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B8" s="24">
-        <v>0.27400000000000002</v>
+        <v>0.245</v>
       </c>
       <c r="C8" s="84">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D8" s="85">
-        <v>0.70512802088869997</v>
+        <v>0.49932887540240001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B9" s="24">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C9" s="84">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D9" s="85">
-        <v>0.58425392870920001</v>
+        <v>0.48964135727449998</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B10" s="24">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C10" s="84">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D10" s="85">
-        <v>0.53227042279350001</v>
+        <v>0.37648172890909998</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="87">
-        <v>14</v>
+      <c r="A11" s="1">
+        <v>6</v>
       </c>
       <c r="B11" s="24">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C11" s="84">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D11" s="85">
-        <v>0.48980424001869999</v>
+        <v>0.32350813634699999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>16</v>
+      <c r="A12" s="87">
+        <v>7</v>
       </c>
       <c r="B12" s="24">
-        <v>0.245</v>
+        <v>0.629</v>
       </c>
       <c r="C12" s="84">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D12" s="85">
-        <v>0.73025348365450005</v>
+        <v>0.27052430519550003</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B13" s="24">
-        <v>0.27400000000000002</v>
+        <v>0.245</v>
       </c>
       <c r="C13" s="84">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="D13" s="85">
-        <v>0.7331210458563</v>
+        <v>0.49518678690250001</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B14" s="24">
-        <v>0.45200000000000001</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C14" s="84">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="D14" s="85">
-        <v>0.58420106096680002</v>
+        <v>0.48483829699800002</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B15" s="24">
-        <v>0.54</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="C15" s="84">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="D15" s="85">
-        <v>0.59116965124190002</v>
+        <v>0.3686266592145</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B16" s="24">
-        <v>0.629</v>
+        <v>0.54</v>
       </c>
       <c r="C16" s="84">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="D16" s="85">
-        <v>0.54492962852030002</v>
+        <v>0.31507954093340002</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
+      <c r="A17" s="1">
+        <v>26</v>
+      </c>
+      <c r="B17" s="24">
+        <v>0.629</v>
+      </c>
+      <c r="C17" s="84">
+        <v>1.25</v>
       </c>
       <c r="D17" s="85">
-        <v>0.56385624898730002</v>
+        <v>0.26111821018469999</v>
       </c>
     </row>
   </sheetData>
@@ -12091,16 +12094,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="7"/>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="102" t="s">
+      <c r="C1" s="129"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="131" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="102"/>
-      <c r="G1" s="103"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="132"/>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">

</xml_diff>

<commit_message>
finished AWEA presentation and plots
</commit_message>
<xml_diff>
--- a/testmatrix.xlsx
+++ b/testmatrix.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="14355" windowHeight="7485" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="test matrix" sheetId="1" r:id="rId1"/>
     <sheet name="tip deflection results" sheetId="3" r:id="rId2"/>
-    <sheet name="cross-section heights" sheetId="2" r:id="rId3"/>
+    <sheet name="root bending moment results" sheetId="4" r:id="rId3"/>
+    <sheet name="cross-section heights" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="72">
   <si>
     <t>test #</t>
   </si>
@@ -371,6 +372,9 @@
   </si>
   <si>
     <t>0 (mono)</t>
+  </si>
+  <si>
+    <t>constload max root bending moment [N*m]</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1036,7 @@
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1374,6 +1378,9 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent1" xfId="5" builtinId="31"/>
@@ -1625,11 +1632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="43596032"/>
-        <c:axId val="43626880"/>
+        <c:axId val="71333376"/>
+        <c:axId val="71335296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43596032"/>
+        <c:axId val="71333376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,7 +1665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43626880"/>
+        <c:crossAx val="71335296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1666,7 +1673,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43626880"/>
+        <c:axId val="71335296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +1703,254 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43596032"/>
+        <c:crossAx val="71333376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'root bending moment results'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test #</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'root bending moment results'!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0 (mono)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'root bending moment results'!$D$2:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4220684.853042</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1927454.796355</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1890012.558225</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1473521.8888089999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1490034.1611820001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1545328.015103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2421609.3755339999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2334918.6731199999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1374347.755192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1415686.3223919999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1495944.842655</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2965386.4971030001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2822496.9016280002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1252281.0428230001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1326247.237337</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1475907.580454</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="93914240"/>
+        <c:axId val="93916160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="93914240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93916160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93916160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>constload tip deflection [m]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93914240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1749,6 +2003,43 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11816,7 +12107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -12072,6 +12363,265 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="86" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="133">
+        <v>4220684.853042</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>9</v>
+      </c>
+      <c r="B3" s="24">
+        <v>0.245</v>
+      </c>
+      <c r="C3" s="84">
+        <v>0.75</v>
+      </c>
+      <c r="D3" s="133">
+        <v>1927454.796355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" s="24">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="C4" s="84">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="133">
+        <v>1890012.558225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" s="24">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="C5" s="84">
+        <v>0.75</v>
+      </c>
+      <c r="D5" s="133">
+        <v>1473521.8888089999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>13</v>
+      </c>
+      <c r="B6" s="24">
+        <v>0.54</v>
+      </c>
+      <c r="C6" s="84">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="133">
+        <v>1490034.1611820001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="87">
+        <v>14</v>
+      </c>
+      <c r="B7" s="24">
+        <v>0.629</v>
+      </c>
+      <c r="C7" s="84">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="133">
+        <v>1545328.015103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="24">
+        <v>0.245</v>
+      </c>
+      <c r="C8" s="84">
+        <v>1</v>
+      </c>
+      <c r="D8" s="133">
+        <v>2421609.3755339999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="24">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="C9" s="84">
+        <v>1</v>
+      </c>
+      <c r="D9" s="133">
+        <v>2334918.6731199999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="24">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="C10" s="84">
+        <v>1</v>
+      </c>
+      <c r="D10" s="133">
+        <v>1374347.755192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="24">
+        <v>0.54</v>
+      </c>
+      <c r="C11" s="84">
+        <v>1</v>
+      </c>
+      <c r="D11" s="133">
+        <v>1415686.3223919999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="87">
+        <v>7</v>
+      </c>
+      <c r="B12" s="24">
+        <v>0.629</v>
+      </c>
+      <c r="C12" s="84">
+        <v>1</v>
+      </c>
+      <c r="D12" s="133">
+        <v>1495944.842655</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>22</v>
+      </c>
+      <c r="B13" s="24">
+        <v>0.245</v>
+      </c>
+      <c r="C13" s="84">
+        <v>1.25</v>
+      </c>
+      <c r="D13" s="133">
+        <v>2965386.4971030001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>23</v>
+      </c>
+      <c r="B14" s="24">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="C14" s="84">
+        <v>1.25</v>
+      </c>
+      <c r="D14" s="133">
+        <v>2822496.9016280002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>24</v>
+      </c>
+      <c r="B15" s="24">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="C15" s="84">
+        <v>1.25</v>
+      </c>
+      <c r="D15" s="133">
+        <v>1252281.0428230001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>25</v>
+      </c>
+      <c r="B16" s="24">
+        <v>0.54</v>
+      </c>
+      <c r="C16" s="84">
+        <v>1.25</v>
+      </c>
+      <c r="D16" s="133">
+        <v>1326247.237337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>26</v>
+      </c>
+      <c r="B17" s="24">
+        <v>0.629</v>
+      </c>
+      <c r="C17" s="84">
+        <v>1.25</v>
+      </c>
+      <c r="D17" s="133">
+        <v>1475907.580454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>

</xml_diff>